<commit_message>
pushing functional trait data, trying gower stuff
</commit_message>
<xml_diff>
--- a/data/functional-traits/joe-traits-lter.xlsx
+++ b/data/functional-traits/joe-traits-lter.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/An/github/algae-traits/data/fong-categorical/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/An/github/functional-responses/data/functional-traits/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB309F99-7554-F541-8180-A5F6010967DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7230ACBB-BEB1-5B41-9B88-F3693ABFEF1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3940" yWindow="500" windowWidth="35420" windowHeight="21060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7140" yWindow="500" windowWidth="35420" windowHeight="21060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="traits" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2585" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2584" uniqueCount="229">
   <si>
     <t>scientific_name</t>
   </si>
@@ -1211,13 +1211,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1604,7 +1603,7 @@
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A8" sqref="A8"/>
-      <selection pane="topRight" activeCell="A28" sqref="A28"/>
+      <selection pane="topRight" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7822,292 +7821,312 @@
         <v>185</v>
       </c>
     </row>
-    <row r="44" spans="1:70" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="5" t="s">
+    <row r="44" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>100</v>
       </c>
-      <c r="B44" s="5">
+      <c r="B44">
         <v>45</v>
       </c>
-      <c r="C44" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H44" s="5" t="s">
+      <c r="C44" t="s">
+        <v>133</v>
+      </c>
+      <c r="D44" t="s">
+        <v>185</v>
+      </c>
+      <c r="E44" t="s">
+        <v>22</v>
+      </c>
+      <c r="F44" t="s">
+        <v>22</v>
+      </c>
+      <c r="G44" t="s">
+        <v>22</v>
+      </c>
+      <c r="H44" t="s">
         <v>34</v>
       </c>
-      <c r="I44" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="J44" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="K44" s="5" t="s">
+      <c r="I44" t="s">
+        <v>133</v>
+      </c>
+      <c r="J44" t="s">
+        <v>185</v>
+      </c>
+      <c r="K44" t="s">
         <v>33</v>
       </c>
-      <c r="L44" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="M44" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="N44" s="5" t="s">
+      <c r="L44" t="s">
+        <v>22</v>
+      </c>
+      <c r="M44" t="s">
+        <v>22</v>
+      </c>
+      <c r="N44" t="s">
         <v>33</v>
       </c>
-      <c r="O44" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="P44" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q44" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="T44" s="5" t="s">
+      <c r="O44" t="s">
+        <v>133</v>
+      </c>
+      <c r="P44" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>32</v>
+      </c>
+      <c r="T44" t="s">
         <v>29</v>
       </c>
-      <c r="U44" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="V44" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="W44" s="5" t="s">
+      <c r="U44" t="s">
+        <v>133</v>
+      </c>
+      <c r="V44" t="s">
+        <v>184</v>
+      </c>
+      <c r="W44" t="s">
         <v>36</v>
       </c>
-      <c r="Z44" s="5" t="s">
+      <c r="Z44" t="s">
         <v>62</v>
       </c>
-      <c r="AC44" s="5" t="s">
+      <c r="AC44" t="s">
         <v>63</v>
       </c>
-      <c r="AF44" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI44" s="5" t="s">
+      <c r="AF44" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI44" t="s">
         <v>61</v>
       </c>
-      <c r="AJ44" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="AK44" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="AL44" s="5" t="s">
+      <c r="AJ44" t="s">
+        <v>133</v>
+      </c>
+      <c r="AK44" t="s">
+        <v>184</v>
+      </c>
+      <c r="AL44" t="s">
         <v>30</v>
       </c>
-      <c r="AM44" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="AN44" s="5" t="s">
+      <c r="AM44" t="s">
+        <v>133</v>
+      </c>
+      <c r="AN44" t="s">
         <v>183</v>
       </c>
-      <c r="AO44" s="5" t="s">
+      <c r="AO44" t="s">
         <v>121</v>
       </c>
-      <c r="AP44" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="AQ44" s="5" t="s">
+      <c r="AP44" t="s">
+        <v>133</v>
+      </c>
+      <c r="AQ44" t="s">
         <v>183</v>
       </c>
-      <c r="AR44" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AU44" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="AX44" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="BA44" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="BD44" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="BG44" s="5" t="s">
+      <c r="AR44" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU44" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV44"/>
+      <c r="AW44"/>
+      <c r="AX44" t="s">
+        <v>22</v>
+      </c>
+      <c r="AY44"/>
+      <c r="AZ44"/>
+      <c r="BA44" t="s">
+        <v>22</v>
+      </c>
+      <c r="BB44"/>
+      <c r="BC44"/>
+      <c r="BD44" t="s">
+        <v>32</v>
+      </c>
+      <c r="BE44"/>
+      <c r="BF44"/>
+      <c r="BG44" t="s">
         <v>64</v>
       </c>
-      <c r="BH44" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="BI44" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="BJ44" s="5" t="s">
+      <c r="BH44" t="s">
+        <v>133</v>
+      </c>
+      <c r="BI44" t="s">
+        <v>185</v>
+      </c>
+      <c r="BJ44" t="s">
         <v>39</v>
       </c>
-      <c r="BK44" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="BL44" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="BM44" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="BP44" s="5" t="s">
+      <c r="BK44" t="s">
+        <v>133</v>
+      </c>
+      <c r="BL44" t="s">
+        <v>185</v>
+      </c>
+      <c r="BM44" t="s">
+        <v>22</v>
+      </c>
+      <c r="BN44"/>
+      <c r="BO44"/>
+      <c r="BP44" t="s">
         <v>189</v>
       </c>
-      <c r="BQ44" s="5" t="s">
+      <c r="BQ44" t="s">
         <v>196</v>
       </c>
-      <c r="BR44" s="5" t="s">
+      <c r="BR44" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="45" spans="1:70" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="5" t="s">
+    <row r="45" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>101</v>
       </c>
-      <c r="B45" s="5">
+      <c r="B45">
         <v>25</v>
       </c>
-      <c r="C45" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="E45" s="5">
+      <c r="C45" t="s">
+        <v>133</v>
+      </c>
+      <c r="D45" t="s">
+        <v>185</v>
+      </c>
+      <c r="E45">
         <v>4</v>
       </c>
-      <c r="F45" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="G45" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="H45" s="5" t="s">
+      <c r="F45" t="s">
+        <v>133</v>
+      </c>
+      <c r="G45" t="s">
+        <v>184</v>
+      </c>
+      <c r="H45" t="s">
         <v>34</v>
       </c>
-      <c r="I45" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="J45" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="K45" s="5" t="s">
+      <c r="I45" t="s">
+        <v>133</v>
+      </c>
+      <c r="J45" t="s">
+        <v>185</v>
+      </c>
+      <c r="K45" t="s">
         <v>33</v>
       </c>
-      <c r="L45" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="N45" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q45" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="T45" s="5" t="s">
+      <c r="L45" t="s">
+        <v>133</v>
+      </c>
+      <c r="N45" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>32</v>
+      </c>
+      <c r="T45" t="s">
         <v>50</v>
       </c>
-      <c r="U45" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="V45" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="W45" s="5" t="s">
+      <c r="U45" t="s">
+        <v>133</v>
+      </c>
+      <c r="V45" t="s">
+        <v>185</v>
+      </c>
+      <c r="W45" t="s">
         <v>54</v>
       </c>
-      <c r="X45" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="Y45" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="Z45" s="5" t="s">
+      <c r="X45" t="s">
+        <v>133</v>
+      </c>
+      <c r="Y45" t="s">
+        <v>184</v>
+      </c>
+      <c r="Z45" t="s">
         <v>35</v>
       </c>
-      <c r="AC45" s="5" t="s">
+      <c r="AC45" t="s">
         <v>37</v>
       </c>
-      <c r="AF45" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI45" s="5" t="s">
+      <c r="AF45" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI45" t="s">
         <v>61</v>
       </c>
-      <c r="AJ45" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="AK45" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="AL45" s="5" t="s">
+      <c r="AJ45" t="s">
+        <v>133</v>
+      </c>
+      <c r="AK45" t="s">
+        <v>184</v>
+      </c>
+      <c r="AL45" t="s">
         <v>30</v>
       </c>
-      <c r="AM45" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="AN45" s="5" t="s">
+      <c r="AM45" t="s">
+        <v>133</v>
+      </c>
+      <c r="AN45" t="s">
         <v>182</v>
       </c>
-      <c r="AO45" s="5" t="s">
+      <c r="AO45" t="s">
         <v>121</v>
       </c>
-      <c r="AP45" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="AQ45" s="5" t="s">
+      <c r="AP45" t="s">
+        <v>133</v>
+      </c>
+      <c r="AQ45" t="s">
         <v>182</v>
       </c>
-      <c r="AR45" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AU45" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="AX45" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="BA45" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="BD45" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="BG45" s="5" t="s">
+      <c r="AR45" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU45" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV45"/>
+      <c r="AW45"/>
+      <c r="AX45" t="s">
+        <v>22</v>
+      </c>
+      <c r="AY45"/>
+      <c r="AZ45"/>
+      <c r="BA45" t="s">
+        <v>22</v>
+      </c>
+      <c r="BB45"/>
+      <c r="BC45"/>
+      <c r="BD45" t="s">
+        <v>32</v>
+      </c>
+      <c r="BE45"/>
+      <c r="BF45"/>
+      <c r="BG45" t="s">
         <v>64</v>
       </c>
-      <c r="BH45" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="BI45" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="BJ45" s="5" t="s">
+      <c r="BH45" t="s">
+        <v>133</v>
+      </c>
+      <c r="BI45" t="s">
+        <v>185</v>
+      </c>
+      <c r="BJ45" t="s">
         <v>39</v>
       </c>
-      <c r="BK45" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="BL45" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="BM45" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="BP45" s="5" t="s">
+      <c r="BK45" t="s">
+        <v>133</v>
+      </c>
+      <c r="BL45" t="s">
+        <v>185</v>
+      </c>
+      <c r="BM45" t="s">
+        <v>22</v>
+      </c>
+      <c r="BN45"/>
+      <c r="BO45"/>
+      <c r="BP45" t="s">
         <v>190</v>
       </c>
-      <c r="BQ45" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="BR45" s="5" t="s">
+      <c r="BQ45" t="s">
+        <v>133</v>
+      </c>
+      <c r="BR45" t="s">
         <v>181</v>
       </c>
     </row>
@@ -8254,271 +8273,295 @@
         <v>185</v>
       </c>
     </row>
-    <row r="47" spans="1:70" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="5" t="s">
+    <row r="47" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>103</v>
       </c>
-      <c r="B47" s="5">
+      <c r="B47">
         <v>11</v>
       </c>
-      <c r="C47" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="E47" s="5">
+      <c r="C47" t="s">
+        <v>133</v>
+      </c>
+      <c r="D47" t="s">
+        <v>185</v>
+      </c>
+      <c r="E47">
         <v>4</v>
       </c>
-      <c r="F47" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="H47" s="5" t="s">
+      <c r="F47" t="s">
+        <v>133</v>
+      </c>
+      <c r="G47" t="s">
+        <v>185</v>
+      </c>
+      <c r="H47" t="s">
         <v>34</v>
       </c>
-      <c r="I47" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="J47" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="K47" s="5" t="s">
+      <c r="I47" t="s">
+        <v>133</v>
+      </c>
+      <c r="J47" t="s">
+        <v>185</v>
+      </c>
+      <c r="K47" t="s">
         <v>33</v>
       </c>
-      <c r="L47" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="N47" s="5" t="s">
+      <c r="L47" t="s">
+        <v>133</v>
+      </c>
+      <c r="N47" t="s">
         <v>33</v>
       </c>
-      <c r="O47" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="P47" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q47" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="T47" s="5" t="s">
+      <c r="O47" t="s">
+        <v>133</v>
+      </c>
+      <c r="P47" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>32</v>
+      </c>
+      <c r="T47" t="s">
         <v>50</v>
       </c>
-      <c r="U47" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="V47" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="W47" s="5" t="s">
+      <c r="U47" t="s">
+        <v>133</v>
+      </c>
+      <c r="V47" t="s">
+        <v>185</v>
+      </c>
+      <c r="W47" t="s">
         <v>36</v>
       </c>
-      <c r="Z47" s="5" t="s">
+      <c r="Z47" t="s">
         <v>62</v>
       </c>
-      <c r="AC47" s="5" t="s">
+      <c r="AC47" t="s">
         <v>63</v>
       </c>
-      <c r="AF47" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI47" s="5" t="s">
+      <c r="AF47" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI47" t="s">
         <v>118</v>
       </c>
-      <c r="AJ47" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="AK47" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="AL47" s="5" t="s">
+      <c r="AJ47" t="s">
+        <v>133</v>
+      </c>
+      <c r="AK47" t="s">
+        <v>185</v>
+      </c>
+      <c r="AL47" t="s">
         <v>30</v>
       </c>
-      <c r="AM47" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="AN47" s="5" t="s">
+      <c r="AM47" t="s">
+        <v>133</v>
+      </c>
+      <c r="AN47" t="s">
         <v>182</v>
       </c>
-      <c r="AO47" s="5" t="s">
+      <c r="AO47" t="s">
         <v>121</v>
       </c>
-      <c r="AP47" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="AQ47" s="5" t="s">
+      <c r="AP47" t="s">
+        <v>133</v>
+      </c>
+      <c r="AQ47" t="s">
         <v>182</v>
       </c>
-      <c r="AR47" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AU47" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="AX47" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="BA47" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="BD47" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="BG47" s="5" t="s">
+      <c r="AR47" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU47" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV47"/>
+      <c r="AW47"/>
+      <c r="AX47" t="s">
+        <v>22</v>
+      </c>
+      <c r="AY47"/>
+      <c r="AZ47"/>
+      <c r="BA47" t="s">
+        <v>22</v>
+      </c>
+      <c r="BB47"/>
+      <c r="BC47"/>
+      <c r="BD47" t="s">
+        <v>32</v>
+      </c>
+      <c r="BE47"/>
+      <c r="BF47"/>
+      <c r="BG47" t="s">
         <v>64</v>
       </c>
-      <c r="BH47" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="BI47" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="BJ47" s="5" t="s">
+      <c r="BH47" t="s">
+        <v>133</v>
+      </c>
+      <c r="BI47" t="s">
+        <v>185</v>
+      </c>
+      <c r="BJ47" t="s">
         <v>39</v>
       </c>
-      <c r="BK47" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="BL47" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="BM47" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="BP47" s="5" t="s">
+      <c r="BK47" t="s">
+        <v>133</v>
+      </c>
+      <c r="BL47" t="s">
+        <v>185</v>
+      </c>
+      <c r="BM47" t="s">
+        <v>22</v>
+      </c>
+      <c r="BN47"/>
+      <c r="BO47"/>
+      <c r="BP47" t="s">
         <v>190</v>
       </c>
-      <c r="BQ47" s="5" t="s">
+      <c r="BQ47" t="s">
         <v>196</v>
       </c>
-      <c r="BR47" s="5" t="s">
+      <c r="BR47" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="48" spans="1:70" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="5" t="s">
+    <row r="48" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>104</v>
       </c>
-      <c r="B48" s="5">
+      <c r="B48">
         <v>25</v>
       </c>
-      <c r="C48" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="E48" s="5">
+      <c r="C48" t="s">
+        <v>133</v>
+      </c>
+      <c r="D48" t="s">
+        <v>185</v>
+      </c>
+      <c r="E48">
         <v>4</v>
       </c>
-      <c r="F48" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="G48" s="5" t="s">
+      <c r="F48" t="s">
+        <v>133</v>
+      </c>
+      <c r="G48" t="s">
         <v>183</v>
       </c>
-      <c r="H48" s="5" t="s">
+      <c r="H48" t="s">
         <v>34</v>
       </c>
-      <c r="I48" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="J48" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="K48" s="5" t="s">
+      <c r="I48" t="s">
+        <v>133</v>
+      </c>
+      <c r="J48" t="s">
+        <v>185</v>
+      </c>
+      <c r="K48" t="s">
         <v>33</v>
       </c>
-      <c r="L48" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="N48" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q48" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="T48" s="5" t="s">
+      <c r="L48" t="s">
+        <v>133</v>
+      </c>
+      <c r="N48" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>32</v>
+      </c>
+      <c r="T48" t="s">
         <v>50</v>
       </c>
-      <c r="U48" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="V48" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="W48" s="5" t="s">
+      <c r="U48" t="s">
+        <v>133</v>
+      </c>
+      <c r="V48" t="s">
+        <v>185</v>
+      </c>
+      <c r="W48" t="s">
         <v>36</v>
       </c>
-      <c r="Z48" s="5" t="s">
+      <c r="Z48" t="s">
         <v>62</v>
       </c>
-      <c r="AC48" s="5" t="s">
+      <c r="AC48" t="s">
         <v>63</v>
       </c>
-      <c r="AF48" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI48" s="5" t="s">
+      <c r="AF48" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI48" t="s">
         <v>61</v>
       </c>
-      <c r="AJ48" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="AK48" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="AL48" s="5" t="s">
+      <c r="AJ48" t="s">
+        <v>133</v>
+      </c>
+      <c r="AK48" t="s">
+        <v>185</v>
+      </c>
+      <c r="AL48" t="s">
         <v>30</v>
       </c>
-      <c r="AM48" s="5" t="s">
+      <c r="AM48" t="s">
         <v>221</v>
       </c>
-      <c r="AN48" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="AO48" s="5" t="s">
+      <c r="AN48" t="s">
+        <v>184</v>
+      </c>
+      <c r="AO48" t="s">
         <v>121</v>
       </c>
-      <c r="AP48" s="5" t="s">
+      <c r="AP48" t="s">
         <v>222</v>
       </c>
-      <c r="AQ48" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="AR48" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AU48" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="AX48" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="BA48" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="BD48" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="BG48" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="BJ48" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="BM48" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="BP48" s="5" t="s">
+      <c r="AQ48" t="s">
+        <v>184</v>
+      </c>
+      <c r="AR48" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU48" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV48"/>
+      <c r="AW48"/>
+      <c r="AX48" t="s">
+        <v>22</v>
+      </c>
+      <c r="AY48"/>
+      <c r="AZ48"/>
+      <c r="BA48" t="s">
+        <v>22</v>
+      </c>
+      <c r="BB48"/>
+      <c r="BC48"/>
+      <c r="BD48" t="s">
+        <v>22</v>
+      </c>
+      <c r="BE48"/>
+      <c r="BF48"/>
+      <c r="BG48" t="s">
+        <v>22</v>
+      </c>
+      <c r="BH48"/>
+      <c r="BI48"/>
+      <c r="BJ48" t="s">
+        <v>22</v>
+      </c>
+      <c r="BK48"/>
+      <c r="BL48"/>
+      <c r="BM48" t="s">
+        <v>22</v>
+      </c>
+      <c r="BN48"/>
+      <c r="BO48"/>
+      <c r="BP48" t="s">
         <v>190</v>
       </c>
-      <c r="BQ48" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="BR48" s="5" t="s">
+      <c r="BQ48" t="s">
+        <v>133</v>
+      </c>
+      <c r="BR48" t="s">
         <v>181</v>
       </c>
     </row>
@@ -8802,693 +8845,741 @@
         <v>185</v>
       </c>
     </row>
-    <row r="51" spans="1:70" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="5" t="s">
+    <row r="51" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>107</v>
       </c>
-      <c r="B51" s="5">
+      <c r="B51">
         <v>15</v>
       </c>
-      <c r="C51" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="E51" s="5">
+      <c r="C51" t="s">
+        <v>133</v>
+      </c>
+      <c r="D51" t="s">
+        <v>185</v>
+      </c>
+      <c r="E51">
         <v>4</v>
       </c>
-      <c r="F51" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="G51" s="5" t="s">
+      <c r="F51" t="s">
+        <v>133</v>
+      </c>
+      <c r="G51" t="s">
         <v>183</v>
       </c>
-      <c r="H51" s="5" t="s">
+      <c r="H51" t="s">
         <v>34</v>
       </c>
-      <c r="I51" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="J51" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="K51" s="5" t="s">
+      <c r="I51" t="s">
+        <v>133</v>
+      </c>
+      <c r="J51" t="s">
+        <v>185</v>
+      </c>
+      <c r="K51" t="s">
         <v>33</v>
       </c>
-      <c r="L51" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="N51" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q51" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="T51" s="5" t="s">
+      <c r="L51" t="s">
+        <v>133</v>
+      </c>
+      <c r="N51" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>32</v>
+      </c>
+      <c r="T51" t="s">
         <v>50</v>
       </c>
-      <c r="U51" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="V51" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="W51" s="5" t="s">
+      <c r="U51" t="s">
+        <v>133</v>
+      </c>
+      <c r="V51" t="s">
+        <v>185</v>
+      </c>
+      <c r="W51" t="s">
         <v>54</v>
       </c>
-      <c r="X51" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="Y51" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="Z51" s="5" t="s">
+      <c r="X51" t="s">
+        <v>133</v>
+      </c>
+      <c r="Y51" t="s">
+        <v>184</v>
+      </c>
+      <c r="Z51" t="s">
         <v>35</v>
       </c>
-      <c r="AC51" s="5" t="s">
+      <c r="AC51" t="s">
         <v>37</v>
       </c>
-      <c r="AF51" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI51" s="5" t="s">
+      <c r="AF51" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI51" t="s">
         <v>61</v>
       </c>
-      <c r="AJ51" s="5" t="s">
+      <c r="AJ51" t="s">
         <v>224</v>
       </c>
-      <c r="AK51" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="AL51" s="5" t="s">
+      <c r="AK51" t="s">
+        <v>184</v>
+      </c>
+      <c r="AL51" t="s">
         <v>30</v>
       </c>
-      <c r="AM51" s="5" t="s">
+      <c r="AM51" t="s">
         <v>224</v>
       </c>
-      <c r="AN51" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="AO51" s="5" t="s">
+      <c r="AN51" t="s">
+        <v>184</v>
+      </c>
+      <c r="AO51" t="s">
         <v>121</v>
       </c>
-      <c r="AP51" s="5" t="s">
+      <c r="AP51" t="s">
         <v>223</v>
       </c>
-      <c r="AQ51" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="AR51" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AU51" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="AX51" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="BA51" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="BD51" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="BG51" s="5" t="s">
+      <c r="AQ51" t="s">
+        <v>184</v>
+      </c>
+      <c r="AR51" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU51" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV51"/>
+      <c r="AW51"/>
+      <c r="AX51" t="s">
+        <v>22</v>
+      </c>
+      <c r="AY51"/>
+      <c r="AZ51"/>
+      <c r="BA51" t="s">
+        <v>22</v>
+      </c>
+      <c r="BB51"/>
+      <c r="BC51"/>
+      <c r="BD51" t="s">
+        <v>32</v>
+      </c>
+      <c r="BE51"/>
+      <c r="BF51"/>
+      <c r="BG51" t="s">
         <v>64</v>
       </c>
-      <c r="BH51" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="BI51" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="BJ51" s="5" t="s">
+      <c r="BH51" t="s">
+        <v>133</v>
+      </c>
+      <c r="BI51" t="s">
+        <v>185</v>
+      </c>
+      <c r="BJ51" t="s">
         <v>39</v>
       </c>
-      <c r="BK51" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="BL51" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="BM51" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="BP51" s="5" t="s">
+      <c r="BK51" t="s">
+        <v>133</v>
+      </c>
+      <c r="BL51" t="s">
+        <v>185</v>
+      </c>
+      <c r="BM51" t="s">
+        <v>22</v>
+      </c>
+      <c r="BN51"/>
+      <c r="BO51"/>
+      <c r="BP51" t="s">
         <v>190</v>
       </c>
-      <c r="BQ51" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="BR51" s="5" t="s">
+      <c r="BQ51" t="s">
+        <v>133</v>
+      </c>
+      <c r="BR51" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="52" spans="1:70" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="5" t="s">
+    <row r="52" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>108</v>
       </c>
-      <c r="B52" s="5">
+      <c r="B52">
         <v>70</v>
       </c>
-      <c r="C52" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="E52" s="5">
+      <c r="C52" t="s">
+        <v>133</v>
+      </c>
+      <c r="D52" t="s">
+        <v>185</v>
+      </c>
+      <c r="E52">
         <v>4</v>
       </c>
-      <c r="F52" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="G52" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="H52" s="5" t="s">
+      <c r="F52" t="s">
+        <v>133</v>
+      </c>
+      <c r="G52" t="s">
+        <v>184</v>
+      </c>
+      <c r="H52" t="s">
         <v>34</v>
       </c>
-      <c r="I52" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="J52" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="K52" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="L52" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="N52" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q52" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="T52" s="5" t="s">
+      <c r="I52" t="s">
+        <v>133</v>
+      </c>
+      <c r="J52" t="s">
+        <v>185</v>
+      </c>
+      <c r="K52" t="s">
+        <v>32</v>
+      </c>
+      <c r="L52" t="s">
+        <v>133</v>
+      </c>
+      <c r="N52" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>32</v>
+      </c>
+      <c r="T52" t="s">
         <v>87</v>
       </c>
-      <c r="W52" s="5" t="s">
+      <c r="W52" t="s">
         <v>37</v>
       </c>
-      <c r="Z52" s="5" t="s">
+      <c r="Z52" t="s">
         <v>35</v>
       </c>
-      <c r="AC52" s="5" t="s">
+      <c r="AC52" t="s">
         <v>37</v>
       </c>
-      <c r="AF52" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="AI52" s="5" t="s">
+      <c r="AF52" t="s">
+        <v>22</v>
+      </c>
+      <c r="AI52" t="s">
         <v>61</v>
       </c>
-      <c r="AJ52" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="AK52" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="AL52" s="5" t="s">
+      <c r="AJ52" t="s">
+        <v>133</v>
+      </c>
+      <c r="AK52" t="s">
+        <v>184</v>
+      </c>
+      <c r="AL52" t="s">
         <v>60</v>
       </c>
-      <c r="AM52" s="5" t="s">
+      <c r="AM52" t="s">
         <v>225</v>
       </c>
-      <c r="AN52" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="AO52" s="5" t="s">
+      <c r="AN52" t="s">
+        <v>185</v>
+      </c>
+      <c r="AO52" t="s">
         <v>208</v>
       </c>
-      <c r="AP52" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="AQ52" s="5" t="s">
+      <c r="AP52" t="s">
+        <v>133</v>
+      </c>
+      <c r="AQ52" t="s">
         <v>182</v>
       </c>
-      <c r="AR52" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AU52" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="AX52" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="BA52" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="BD52" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="BG52" s="5" t="s">
+      <c r="AR52" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU52" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV52"/>
+      <c r="AW52"/>
+      <c r="AX52" t="s">
+        <v>22</v>
+      </c>
+      <c r="AY52"/>
+      <c r="AZ52"/>
+      <c r="BA52" t="s">
+        <v>22</v>
+      </c>
+      <c r="BB52"/>
+      <c r="BC52"/>
+      <c r="BD52" t="s">
+        <v>32</v>
+      </c>
+      <c r="BE52"/>
+      <c r="BF52"/>
+      <c r="BG52" t="s">
         <v>64</v>
       </c>
-      <c r="BH52" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="BI52" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="BJ52" s="5" t="s">
+      <c r="BH52" t="s">
+        <v>133</v>
+      </c>
+      <c r="BI52" t="s">
+        <v>185</v>
+      </c>
+      <c r="BJ52" t="s">
         <v>39</v>
       </c>
-      <c r="BK52" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="BL52" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="BM52" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="BP52" s="5" t="s">
+      <c r="BK52" t="s">
+        <v>133</v>
+      </c>
+      <c r="BL52" t="s">
+        <v>185</v>
+      </c>
+      <c r="BM52" t="s">
+        <v>22</v>
+      </c>
+      <c r="BN52"/>
+      <c r="BO52"/>
+      <c r="BP52" t="s">
         <v>190</v>
       </c>
-      <c r="BQ52" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="BR52" s="5" t="s">
+      <c r="BQ52" t="s">
+        <v>133</v>
+      </c>
+      <c r="BR52" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="53" spans="1:70" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="5" t="s">
+    <row r="53" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>109</v>
       </c>
-      <c r="B53" s="5">
+      <c r="B53">
         <v>20</v>
       </c>
-      <c r="C53" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="E53" s="5">
+      <c r="C53" t="s">
+        <v>133</v>
+      </c>
+      <c r="D53" t="s">
+        <v>184</v>
+      </c>
+      <c r="E53">
         <v>4</v>
       </c>
-      <c r="F53" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="G53" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="H53" s="5" t="s">
+      <c r="F53" t="s">
+        <v>133</v>
+      </c>
+      <c r="G53" t="s">
+        <v>184</v>
+      </c>
+      <c r="H53" t="s">
         <v>34</v>
       </c>
-      <c r="I53" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="J53" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="K53" s="5" t="s">
+      <c r="I53" t="s">
+        <v>133</v>
+      </c>
+      <c r="J53" t="s">
+        <v>185</v>
+      </c>
+      <c r="K53" t="s">
         <v>33</v>
       </c>
-      <c r="L53" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="N53" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q53" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="T53" s="5" t="s">
+      <c r="L53" t="s">
+        <v>133</v>
+      </c>
+      <c r="N53" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>32</v>
+      </c>
+      <c r="T53" t="s">
         <v>50</v>
       </c>
-      <c r="U53" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="V53" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="W53" s="5" t="s">
+      <c r="U53" t="s">
+        <v>133</v>
+      </c>
+      <c r="V53" t="s">
+        <v>184</v>
+      </c>
+      <c r="W53" t="s">
         <v>36</v>
       </c>
-      <c r="Z53" s="5" t="s">
+      <c r="Z53" t="s">
         <v>62</v>
       </c>
-      <c r="AC53" s="5" t="s">
+      <c r="AC53" t="s">
         <v>63</v>
       </c>
-      <c r="AF53" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI53" s="5" t="s">
+      <c r="AF53" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI53" t="s">
         <v>61</v>
       </c>
-      <c r="AJ53" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="AK53" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="AL53" s="5" t="s">
+      <c r="AJ53" t="s">
+        <v>133</v>
+      </c>
+      <c r="AK53" t="s">
+        <v>184</v>
+      </c>
+      <c r="AL53" t="s">
         <v>30</v>
       </c>
-      <c r="AM53" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="AN53" s="5" t="s">
+      <c r="AM53" t="s">
+        <v>133</v>
+      </c>
+      <c r="AN53" t="s">
         <v>182</v>
       </c>
-      <c r="AO53" s="5" t="s">
+      <c r="AO53" t="s">
         <v>121</v>
       </c>
-      <c r="AP53" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="AQ53" s="5" t="s">
+      <c r="AP53" t="s">
+        <v>133</v>
+      </c>
+      <c r="AQ53" t="s">
         <v>182</v>
       </c>
-      <c r="AR53" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AU53" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="AX53" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="BA53" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="BD53" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="BG53" s="5" t="s">
+      <c r="AR53" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU53" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV53"/>
+      <c r="AW53"/>
+      <c r="AX53" t="s">
+        <v>22</v>
+      </c>
+      <c r="AY53"/>
+      <c r="AZ53"/>
+      <c r="BA53" t="s">
+        <v>22</v>
+      </c>
+      <c r="BB53"/>
+      <c r="BC53"/>
+      <c r="BD53" t="s">
+        <v>32</v>
+      </c>
+      <c r="BE53"/>
+      <c r="BF53"/>
+      <c r="BG53" t="s">
         <v>64</v>
       </c>
-      <c r="BH53" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="BI53" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="BJ53" s="5" t="s">
+      <c r="BH53" t="s">
+        <v>133</v>
+      </c>
+      <c r="BI53" t="s">
+        <v>185</v>
+      </c>
+      <c r="BJ53" t="s">
         <v>39</v>
       </c>
-      <c r="BK53" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="BL53" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="BM53" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="BP53" s="5" t="s">
+      <c r="BK53" t="s">
+        <v>133</v>
+      </c>
+      <c r="BL53" t="s">
+        <v>185</v>
+      </c>
+      <c r="BM53" t="s">
+        <v>22</v>
+      </c>
+      <c r="BN53"/>
+      <c r="BO53"/>
+      <c r="BP53" t="s">
         <v>190</v>
       </c>
-      <c r="BQ53" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="BR53" s="5" t="s">
+      <c r="BQ53" t="s">
+        <v>133</v>
+      </c>
+      <c r="BR53" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="54" spans="1:70" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="5" t="s">
+    <row r="54" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>110</v>
       </c>
-      <c r="B54" s="5">
+      <c r="B54">
         <v>90</v>
       </c>
-      <c r="C54" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="E54" s="5">
+      <c r="C54" t="s">
+        <v>133</v>
+      </c>
+      <c r="D54" t="s">
+        <v>185</v>
+      </c>
+      <c r="E54">
         <v>4</v>
       </c>
-      <c r="F54" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="G54" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="H54" s="5" t="s">
+      <c r="F54" t="s">
+        <v>133</v>
+      </c>
+      <c r="G54" t="s">
+        <v>184</v>
+      </c>
+      <c r="H54" t="s">
         <v>34</v>
       </c>
-      <c r="I54" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="J54" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="K54" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="N54" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q54" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="R54" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="S54" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="T54" s="5" t="s">
+      <c r="I54" t="s">
+        <v>133</v>
+      </c>
+      <c r="J54" t="s">
+        <v>185</v>
+      </c>
+      <c r="K54" t="s">
+        <v>32</v>
+      </c>
+      <c r="N54" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>32</v>
+      </c>
+      <c r="R54" t="s">
+        <v>133</v>
+      </c>
+      <c r="S54" t="s">
+        <v>184</v>
+      </c>
+      <c r="T54" t="s">
         <v>87</v>
       </c>
-      <c r="W54" s="5" t="s">
+      <c r="W54" t="s">
         <v>37</v>
       </c>
-      <c r="Z54" s="5" t="s">
+      <c r="Z54" t="s">
         <v>62</v>
       </c>
-      <c r="AC54" s="5" t="s">
+      <c r="AC54" t="s">
         <v>63</v>
       </c>
-      <c r="AF54" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI54" s="5" t="s">
+      <c r="AF54" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI54" t="s">
         <v>73</v>
       </c>
-      <c r="AJ54" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="AK54" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="AL54" s="5" t="s">
+      <c r="AJ54" t="s">
+        <v>133</v>
+      </c>
+      <c r="AK54" t="s">
+        <v>185</v>
+      </c>
+      <c r="AL54" t="s">
         <v>60</v>
       </c>
-      <c r="AM54" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="AN54" s="5" t="s">
+      <c r="AM54" t="s">
+        <v>133</v>
+      </c>
+      <c r="AN54" t="s">
         <v>182</v>
       </c>
-      <c r="AO54" s="5" t="s">
+      <c r="AO54" t="s">
         <v>121</v>
       </c>
-      <c r="AP54" s="5" t="s">
+      <c r="AP54" t="s">
         <v>226</v>
       </c>
-      <c r="AQ54" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="AR54" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AU54" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="AX54" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="BA54" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="BD54" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="BG54" s="5" t="s">
+      <c r="AQ54" t="s">
+        <v>184</v>
+      </c>
+      <c r="AR54" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU54" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV54"/>
+      <c r="AW54"/>
+      <c r="AX54" t="s">
+        <v>22</v>
+      </c>
+      <c r="AY54"/>
+      <c r="AZ54"/>
+      <c r="BA54" t="s">
+        <v>22</v>
+      </c>
+      <c r="BB54"/>
+      <c r="BC54"/>
+      <c r="BD54" t="s">
+        <v>32</v>
+      </c>
+      <c r="BE54"/>
+      <c r="BF54"/>
+      <c r="BG54" t="s">
         <v>64</v>
       </c>
-      <c r="BH54" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="BI54" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="BJ54" s="5" t="s">
+      <c r="BH54" t="s">
+        <v>133</v>
+      </c>
+      <c r="BI54" t="s">
+        <v>185</v>
+      </c>
+      <c r="BJ54" t="s">
         <v>39</v>
       </c>
-      <c r="BK54" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="BL54" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="BM54" s="5" t="s">
+      <c r="BK54" t="s">
+        <v>133</v>
+      </c>
+      <c r="BL54" t="s">
+        <v>185</v>
+      </c>
+      <c r="BM54" t="s">
         <v>70</v>
       </c>
-      <c r="BN54" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="BO54" s="5" t="s">
+      <c r="BN54" t="s">
+        <v>133</v>
+      </c>
+      <c r="BO54" t="s">
         <v>182</v>
       </c>
-      <c r="BP54" s="5" t="s">
+      <c r="BP54" t="s">
         <v>190</v>
       </c>
-      <c r="BQ54" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="BR54" s="5" t="s">
+      <c r="BQ54" t="s">
+        <v>133</v>
+      </c>
+      <c r="BR54" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="55" spans="1:70" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="5" t="s">
+    <row r="55" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>111</v>
       </c>
-      <c r="B55" s="5">
+      <c r="B55">
         <v>2</v>
       </c>
-      <c r="C55" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G55" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H55" s="5" t="s">
+      <c r="C55" t="s">
+        <v>133</v>
+      </c>
+      <c r="D55" t="s">
+        <v>185</v>
+      </c>
+      <c r="E55" t="s">
+        <v>22</v>
+      </c>
+      <c r="F55" t="s">
+        <v>22</v>
+      </c>
+      <c r="G55" t="s">
+        <v>22</v>
+      </c>
+      <c r="H55" t="s">
         <v>34</v>
       </c>
-      <c r="K55" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="L55" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="M55" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="N55" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q55" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="T55" s="5" t="s">
+      <c r="K55" t="s">
+        <v>32</v>
+      </c>
+      <c r="L55" t="s">
+        <v>22</v>
+      </c>
+      <c r="M55" t="s">
+        <v>22</v>
+      </c>
+      <c r="N55" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>32</v>
+      </c>
+      <c r="T55" t="s">
         <v>87</v>
       </c>
-      <c r="W55" s="5" t="s">
+      <c r="W55" t="s">
         <v>37</v>
       </c>
-      <c r="Z55" s="5" t="s">
+      <c r="Z55" t="s">
         <v>62</v>
       </c>
-      <c r="AC55" s="5" t="s">
+      <c r="AC55" t="s">
         <v>63</v>
       </c>
-      <c r="AF55" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AG55" s="5" t="s">
+      <c r="AF55" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG55" t="s">
         <v>227</v>
       </c>
-      <c r="AH55" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="AI55" s="5" t="s">
+      <c r="AH55" t="s">
+        <v>184</v>
+      </c>
+      <c r="AI55" t="s">
         <v>73</v>
       </c>
-      <c r="AJ55" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="AK55" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="AL55" s="5" t="s">
+      <c r="AJ55" t="s">
+        <v>133</v>
+      </c>
+      <c r="AK55" t="s">
+        <v>184</v>
+      </c>
+      <c r="AL55" t="s">
         <v>60</v>
       </c>
-      <c r="AM55" s="5" t="s">
+      <c r="AM55" t="s">
         <v>227</v>
       </c>
-      <c r="AN55" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="AO55" s="5" t="s">
+      <c r="AN55" t="s">
+        <v>184</v>
+      </c>
+      <c r="AO55" t="s">
         <v>120</v>
       </c>
-      <c r="AP55" s="5" t="s">
+      <c r="AP55" t="s">
         <v>228</v>
       </c>
-      <c r="AQ55" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="AR55" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AU55" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="AX55" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="BA55" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="BD55" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="BG55" s="5" t="s">
+      <c r="AQ55" t="s">
+        <v>184</v>
+      </c>
+      <c r="AR55" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU55" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV55"/>
+      <c r="AW55"/>
+      <c r="AX55" t="s">
+        <v>22</v>
+      </c>
+      <c r="AY55"/>
+      <c r="AZ55"/>
+      <c r="BA55" t="s">
+        <v>22</v>
+      </c>
+      <c r="BB55"/>
+      <c r="BC55"/>
+      <c r="BD55" t="s">
+        <v>32</v>
+      </c>
+      <c r="BE55"/>
+      <c r="BF55"/>
+      <c r="BG55" t="s">
         <v>64</v>
       </c>
-      <c r="BH55" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="BI55" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="BJ55" s="5" t="s">
+      <c r="BH55" t="s">
+        <v>133</v>
+      </c>
+      <c r="BI55" t="s">
+        <v>184</v>
+      </c>
+      <c r="BJ55" t="s">
         <v>39</v>
       </c>
-      <c r="BK55" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="BL55" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="BM55" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="BP55" s="5" t="s">
+      <c r="BK55" t="s">
+        <v>133</v>
+      </c>
+      <c r="BL55" t="s">
+        <v>184</v>
+      </c>
+      <c r="BM55" t="s">
+        <v>22</v>
+      </c>
+      <c r="BN55"/>
+      <c r="BO55"/>
+      <c r="BP55" t="s">
         <v>191</v>
       </c>
-      <c r="BQ55" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="BR55" s="5" t="s">
+      <c r="BQ55" t="s">
+        <v>133</v>
+      </c>
+      <c r="BR55" t="s">
         <v>184</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD3 A4:AT5 AU4:XFD14 A6:B6 E6:AT6 A7:AT14 AV36:BP38 BS36:XFD38 AV39:XFD40 AV41:BP41 BS41:XFD41 AV42:XFD42 AV43:BP43 BR43:XFD43 AV44:XFD55 A56:XFD1048576 A16:AU55 AV16:XFD35 A15:XFD15">
+  <conditionalFormatting sqref="A1:XFD3 A4:AT5 AU4:XFD14 A6:B6 E6:AT6 A7:AT14 A15:XFD15 AV16:XFD35 A16:AU55 AV36:BP38 BS36:XFD38 AV39:XFD40 AV41:BP41 BS41:XFD41 AV42:XFD42 AV43:BP43 BR43:XFD43 AV44:XFD55 A56:XFD1048576">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
@@ -9658,7 +9749,7 @@
   <dimension ref="A1:X31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V30" sqref="V30"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10133,81 +10224,78 @@
         <v>213</v>
       </c>
     </row>
-    <row r="17" spans="22:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="22:22" x14ac:dyDescent="0.2">
       <c r="V17" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="18" spans="22:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="22:22" x14ac:dyDescent="0.2">
       <c r="V18" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="19" spans="22:23" x14ac:dyDescent="0.2">
+    <row r="19" spans="22:22" x14ac:dyDescent="0.2">
       <c r="V19" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="20" spans="22:23" x14ac:dyDescent="0.2">
+    <row r="20" spans="22:22" x14ac:dyDescent="0.2">
       <c r="V20" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="21" spans="22:23" x14ac:dyDescent="0.2">
+    <row r="21" spans="22:22" x14ac:dyDescent="0.2">
       <c r="V21" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="22" spans="22:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="22:22" x14ac:dyDescent="0.2">
       <c r="V22" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="23" spans="22:23" x14ac:dyDescent="0.2">
+    <row r="23" spans="22:22" x14ac:dyDescent="0.2">
       <c r="V23" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="24" spans="22:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="22:22" x14ac:dyDescent="0.2">
       <c r="V24" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="25" spans="22:23" x14ac:dyDescent="0.2">
+    <row r="25" spans="22:22" x14ac:dyDescent="0.2">
       <c r="V25" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="26" spans="22:23" x14ac:dyDescent="0.2">
+    <row r="26" spans="22:22" x14ac:dyDescent="0.2">
       <c r="V26" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="27" spans="22:23" x14ac:dyDescent="0.2">
+    <row r="27" spans="22:22" x14ac:dyDescent="0.2">
       <c r="V27" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="28" spans="22:23" x14ac:dyDescent="0.2">
+    <row r="28" spans="22:22" x14ac:dyDescent="0.2">
       <c r="V28" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="29" spans="22:23" x14ac:dyDescent="0.2">
+    <row r="29" spans="22:22" x14ac:dyDescent="0.2">
       <c r="V29" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="30" spans="22:23" x14ac:dyDescent="0.2">
+    <row r="30" spans="22:22" x14ac:dyDescent="0.2">
       <c r="V30" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="31" spans="22:23" x14ac:dyDescent="0.2">
+    <row r="31" spans="22:22" x14ac:dyDescent="0.2">
       <c r="V31" t="s">
-        <v>22</v>
-      </c>
-      <c r="W31" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
the clustering...... it is not working.......
</commit_message>
<xml_diff>
--- a/data/functional-traits/joe-traits-lter.xlsx
+++ b/data/functional-traits/joe-traits-lter.xlsx
@@ -1,28 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/An/github/functional-responses/data/functional-traits/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7230ACBB-BEB1-5B41-9B88-F3693ABFEF1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E136B80-044A-C74A-81E5-C5ABD86C1F6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7140" yWindow="500" windowWidth="35420" windowHeight="21060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1640" yWindow="500" windowWidth="35420" windowHeight="21060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="traits" sheetId="1" r:id="rId1"/>
     <sheet name="validation" sheetId="2" r:id="rId2"/>
     <sheet name="validation-notes" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">traits!$A$1:$BR$55</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2584" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2613" uniqueCount="234">
   <si>
     <t>scientific_name</t>
   </si>
@@ -709,6 +712,21 @@
   </si>
   <si>
     <t>Choi, T.-S., E.-J. Kang, J.-H. Kim, and K.-Y. Kim. 2010. Effect of salinity on growth and nutrient uptake of Ulva pertusa (Chlorophyta) from an eelgrass bed. ALGAE 25:17–26.</t>
+  </si>
+  <si>
+    <t>Hughey, J. R., and M. H. Hommersand. 2008. Morphological and molecular systematic study of Chondracanthus (Gigartinaceae, Rhodophyta) from Pacific North America. Phycologia 47:124–155.</t>
+  </si>
+  <si>
+    <t>Katsaros, C. I. 1995. Apical cells of brown algae with particular reference to Sphacelariales, Dictyotales and Fucales. Phycological Research 43:43–59.</t>
+  </si>
+  <si>
+    <t>Harvey, A. S., W. J. Woelkerling, and A. J. K. Millar. 2009. The genus Amphiroa (Lithophylloideae, Corallinaceae, Rhodophyta) from the temperate coasts of the Australian continent, including the newly described A. klochkovana. Phycologia 48:258–290.</t>
+  </si>
+  <si>
+    <t>Dolan, S. 2001. The use of medullary unit patterns of intergenicula and genicula in the taxonomy of Amphiroa (Corallinaceae, Rhodophyta). European Journal of Phycology 36:397–407.</t>
+  </si>
+  <si>
+    <t>Gorostiaga, J. M. 1994. Growth and production of the red alga Gelidium sesquipedale off the Basque coast (northern Spain). Marine Biology 120:311–322.</t>
   </si>
 </sst>
 </file>
@@ -1601,14 +1619,15 @@
   <dimension ref="A1:BR55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="Z1" activePane="topRight" state="frozen"/>
       <selection activeCell="A8" sqref="A8"/>
-      <selection pane="topRight" activeCell="C7" sqref="C7"/>
+      <selection pane="topRight" activeCell="AR30" sqref="AR30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="53.83203125" customWidth="1"/>
+    <col min="13" max="43" width="10.83203125" customWidth="1"/>
     <col min="47" max="70" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
@@ -1834,8 +1853,8 @@
       <c r="C2" t="s">
         <v>133</v>
       </c>
-      <c r="E2" t="s">
-        <v>22</v>
+      <c r="E2">
+        <v>4</v>
       </c>
       <c r="F2" t="s">
         <v>22</v>
@@ -1859,37 +1878,61 @@
         <v>133</v>
       </c>
       <c r="N2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="Q2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="T2" t="s">
-        <v>22</v>
+        <v>29</v>
+      </c>
+      <c r="U2" t="s">
+        <v>133</v>
+      </c>
+      <c r="V2" t="s">
+        <v>184</v>
       </c>
       <c r="W2" t="s">
-        <v>22</v>
+        <v>36</v>
+      </c>
+      <c r="X2" t="s">
+        <v>231</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>185</v>
       </c>
       <c r="Z2" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="AC2" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="AF2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="AI2" t="s">
-        <v>22</v>
+        <v>31</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>133</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>184</v>
       </c>
       <c r="AL2" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="AO2" t="s">
-        <v>22</v>
+        <v>208</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>232</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>184</v>
       </c>
       <c r="AR2" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="AU2" t="s">
         <v>22</v>
@@ -1968,7 +2011,7 @@
         <v>185</v>
       </c>
       <c r="K3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L3" t="s">
         <v>133</v>
@@ -2154,7 +2197,7 @@
         <v>185</v>
       </c>
       <c r="K4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L4" t="s">
         <v>155</v>
@@ -2309,8 +2352,8 @@
       <c r="C5" t="s">
         <v>155</v>
       </c>
-      <c r="E5" t="s">
-        <v>22</v>
+      <c r="E5">
+        <v>4</v>
       </c>
       <c r="F5" t="s">
         <v>22</v>
@@ -2328,7 +2371,7 @@
         <v>185</v>
       </c>
       <c r="K5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N5" t="s">
         <v>32</v>
@@ -2895,14 +2938,14 @@
       <c r="C9" t="s">
         <v>133</v>
       </c>
-      <c r="E9" t="s">
-        <v>22</v>
+      <c r="E9">
+        <v>4</v>
       </c>
       <c r="F9" t="s">
-        <v>22</v>
+        <v>133</v>
       </c>
       <c r="G9" t="s">
-        <v>22</v>
+        <v>184</v>
       </c>
       <c r="H9" t="s">
         <v>34</v>
@@ -2914,40 +2957,64 @@
         <v>183</v>
       </c>
       <c r="K9" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="N9" t="s">
-        <v>22</v>
+        <v>33</v>
+      </c>
+      <c r="O9" t="s">
+        <v>229</v>
+      </c>
+      <c r="P9" t="s">
+        <v>184</v>
       </c>
       <c r="Q9" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="T9" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="W9" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="Z9" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="AC9" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="AF9" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="AI9" t="s">
-        <v>22</v>
+        <v>61</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>133</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>184</v>
       </c>
       <c r="AL9" t="s">
-        <v>22</v>
+        <v>30</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>133</v>
+      </c>
+      <c r="AN9" t="s">
+        <v>184</v>
       </c>
       <c r="AO9" t="s">
-        <v>22</v>
+        <v>121</v>
+      </c>
+      <c r="AP9" t="s">
+        <v>229</v>
+      </c>
+      <c r="AQ9" t="s">
+        <v>184</v>
       </c>
       <c r="AR9" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="AU9" s="2" t="s">
         <v>22</v>
@@ -2959,13 +3026,25 @@
         <v>22</v>
       </c>
       <c r="BD9" s="2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="BG9" s="2" t="s">
-        <v>22</v>
+        <v>64</v>
+      </c>
+      <c r="BH9" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="BI9" s="2" t="s">
+        <v>185</v>
       </c>
       <c r="BJ9" s="2" t="s">
-        <v>22</v>
+        <v>39</v>
+      </c>
+      <c r="BK9" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="BL9" s="2" t="s">
+        <v>184</v>
       </c>
       <c r="BM9" s="2" t="s">
         <v>22</v>
@@ -3012,7 +3091,7 @@
         <v>183</v>
       </c>
       <c r="K10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L10" t="s">
         <v>155</v>
@@ -3173,8 +3252,8 @@
       <c r="D11" t="s">
         <v>185</v>
       </c>
-      <c r="E11" t="s">
-        <v>22</v>
+      <c r="E11">
+        <v>4</v>
       </c>
       <c r="F11" t="s">
         <v>22</v>
@@ -3192,7 +3271,7 @@
         <v>184</v>
       </c>
       <c r="K11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L11" t="s">
         <v>133</v>
@@ -3698,7 +3777,7 @@
         <v>22</v>
       </c>
       <c r="AI14" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="AL14" t="s">
         <v>51</v>
@@ -3780,8 +3859,8 @@
       <c r="C15" t="s">
         <v>155</v>
       </c>
-      <c r="E15" t="s">
-        <v>22</v>
+      <c r="E15">
+        <v>4</v>
       </c>
       <c r="F15" t="s">
         <v>22</v>
@@ -3799,7 +3878,7 @@
         <v>185</v>
       </c>
       <c r="K15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N15" t="s">
         <v>32</v>
@@ -4107,7 +4186,7 @@
         <v>183</v>
       </c>
       <c r="K17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L17" t="s">
         <v>155</v>
@@ -4143,7 +4222,7 @@
         <v>91</v>
       </c>
       <c r="AF17" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="AI17" t="s">
         <v>61</v>
@@ -4384,14 +4463,14 @@
       <c r="D19" t="s">
         <v>185</v>
       </c>
-      <c r="E19" t="s">
-        <v>22</v>
+      <c r="E19">
+        <v>4</v>
       </c>
       <c r="F19" t="s">
-        <v>22</v>
+        <v>133</v>
       </c>
       <c r="G19" t="s">
-        <v>22</v>
+        <v>185</v>
       </c>
       <c r="H19" t="s">
         <v>34</v>
@@ -4403,43 +4482,67 @@
         <v>184</v>
       </c>
       <c r="K19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L19" t="s">
         <v>133</v>
       </c>
       <c r="N19" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="Q19" t="s">
-        <v>22</v>
+        <v>32</v>
+      </c>
+      <c r="R19" t="s">
+        <v>133</v>
+      </c>
+      <c r="S19" t="s">
+        <v>184</v>
       </c>
       <c r="T19" t="s">
-        <v>22</v>
+        <v>50</v>
+      </c>
+      <c r="U19" t="s">
+        <v>133</v>
+      </c>
+      <c r="V19" t="s">
+        <v>184</v>
       </c>
       <c r="W19" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="Z19" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="AC19" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="AF19" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="AI19" t="s">
-        <v>22</v>
+        <v>118</v>
+      </c>
+      <c r="AJ19" t="s">
+        <v>133</v>
+      </c>
+      <c r="AK19" t="s">
+        <v>184</v>
       </c>
       <c r="AL19" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="AO19" t="s">
-        <v>22</v>
+        <v>121</v>
+      </c>
+      <c r="AP19" t="s">
+        <v>230</v>
+      </c>
+      <c r="AQ19" t="s">
+        <v>183</v>
       </c>
       <c r="AR19" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="AU19" s="2" t="s">
         <v>22</v>
@@ -4451,13 +4554,25 @@
         <v>22</v>
       </c>
       <c r="BD19" s="2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="BG19" s="2" t="s">
-        <v>22</v>
+        <v>64</v>
+      </c>
+      <c r="BH19" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="BI19" s="2" t="s">
+        <v>184</v>
       </c>
       <c r="BJ19" s="2" t="s">
-        <v>22</v>
+        <v>39</v>
+      </c>
+      <c r="BK19" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="BL19" s="2" t="s">
+        <v>184</v>
       </c>
       <c r="BM19" s="2" t="s">
         <v>22</v>
@@ -4641,7 +4756,7 @@
         <v>185</v>
       </c>
       <c r="K21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L21" t="s">
         <v>133</v>
@@ -4701,7 +4816,7 @@
         <v>185</v>
       </c>
       <c r="AF21" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="AI21" t="s">
         <v>90</v>
@@ -4902,7 +5017,7 @@
         <v>185</v>
       </c>
       <c r="K23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L23" t="s">
         <v>133</v>
@@ -4956,7 +5071,7 @@
         <v>131</v>
       </c>
       <c r="AF23" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="AI23" t="s">
         <v>90</v>
@@ -5048,8 +5163,8 @@
       <c r="D24" t="s">
         <v>184</v>
       </c>
-      <c r="E24" t="s">
-        <v>22</v>
+      <c r="E24">
+        <v>4</v>
       </c>
       <c r="F24" t="s">
         <v>22</v>
@@ -5217,7 +5332,7 @@
         <v>184</v>
       </c>
       <c r="K25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L25" t="s">
         <v>133</v>
@@ -5655,7 +5770,7 @@
         <v>184</v>
       </c>
       <c r="K29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L29" t="s">
         <v>133</v>
@@ -5750,7 +5865,7 @@
         <v>184</v>
       </c>
       <c r="K30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L30" t="s">
         <v>133</v>
@@ -5786,16 +5901,22 @@
         <v>37</v>
       </c>
       <c r="AF30" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="AI30" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="AL30" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="AO30" t="s">
-        <v>22</v>
+        <v>121</v>
+      </c>
+      <c r="AP30" t="s">
+        <v>233</v>
+      </c>
+      <c r="AQ30" t="s">
+        <v>184</v>
       </c>
       <c r="AR30" t="s">
         <v>32</v>
@@ -5899,7 +6020,7 @@
         <v>184</v>
       </c>
       <c r="K31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L31" t="s">
         <v>133</v>
@@ -6060,8 +6181,8 @@
       <c r="D32" t="s">
         <v>184</v>
       </c>
-      <c r="E32" t="s">
-        <v>22</v>
+      <c r="E32">
+        <v>4</v>
       </c>
       <c r="F32" t="s">
         <v>22</v>
@@ -6079,7 +6200,7 @@
         <v>184</v>
       </c>
       <c r="K32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L32" t="s">
         <v>133</v>
@@ -6402,7 +6523,7 @@
         <v>184</v>
       </c>
       <c r="K34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L34" t="s">
         <v>133</v>
@@ -6853,7 +6974,7 @@
         <v>184</v>
       </c>
       <c r="K37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L37" t="s">
         <v>133</v>
@@ -7272,7 +7393,7 @@
         <v>185</v>
       </c>
       <c r="K40" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L40" t="s">
         <v>133</v>
@@ -7317,7 +7438,7 @@
         <v>32</v>
       </c>
       <c r="AI40" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="AL40" t="s">
         <v>30</v>
@@ -7417,7 +7538,7 @@
         <v>185</v>
       </c>
       <c r="K41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L41" t="s">
         <v>133</v>
@@ -7548,7 +7669,7 @@
         <v>185</v>
       </c>
       <c r="K42" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L42" t="s">
         <v>133</v>
@@ -7834,8 +7955,8 @@
       <c r="D44" t="s">
         <v>185</v>
       </c>
-      <c r="E44" t="s">
-        <v>22</v>
+      <c r="E44">
+        <v>4</v>
       </c>
       <c r="F44" t="s">
         <v>22</v>
@@ -7853,7 +7974,7 @@
         <v>185</v>
       </c>
       <c r="K44" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L44" t="s">
         <v>22</v>
@@ -8009,7 +8130,7 @@
         <v>185</v>
       </c>
       <c r="K45" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L45" t="s">
         <v>133</v>
@@ -8305,7 +8426,7 @@
         <v>185</v>
       </c>
       <c r="K47" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L47" t="s">
         <v>133</v>
@@ -8458,7 +8579,7 @@
         <v>185</v>
       </c>
       <c r="K48" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L48" t="s">
         <v>133</v>
@@ -8877,7 +8998,7 @@
         <v>185</v>
       </c>
       <c r="K51" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L51" t="s">
         <v>133</v>
@@ -9054,7 +9175,7 @@
         <v>37</v>
       </c>
       <c r="AF52" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="AI52" t="s">
         <v>61</v>
@@ -9171,7 +9292,7 @@
         <v>185</v>
       </c>
       <c r="K53" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L53" t="s">
         <v>133</v>
@@ -9447,8 +9568,8 @@
       <c r="D55" t="s">
         <v>185</v>
       </c>
-      <c r="E55" t="s">
-        <v>22</v>
+      <c r="E55">
+        <v>4</v>
       </c>
       <c r="F55" t="s">
         <v>22</v>
@@ -9579,6 +9700,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:BR55" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="A1:XFD3 A4:AT5 AU4:XFD14 A6:B6 E6:AT6 A7:AT14 A15:XFD15 AV16:XFD35 A16:AU55 AV36:BP38 BS36:XFD38 AV39:XFD40 AV41:BP41 BS41:XFD41 AV42:XFD42 AV43:BP43 BR43:XFD43 AV44:XFD55 A56:XFD1048576">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"NA"</formula>
@@ -9746,10 +9868,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAABEA72-4450-9143-B9EE-F8CB7C81A2E6}">
-  <dimension ref="A1:X31"/>
+  <dimension ref="A1:X38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="V35" sqref="V35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10291,11 +10413,36 @@
     </row>
     <row r="30" spans="22:22" x14ac:dyDescent="0.2">
       <c r="V30" t="s">
-        <v>205</v>
+        <v>229</v>
       </c>
     </row>
     <row r="31" spans="22:22" x14ac:dyDescent="0.2">
       <c r="V31" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="32" spans="22:22" x14ac:dyDescent="0.2">
+      <c r="V32" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="33" spans="22:22" x14ac:dyDescent="0.2">
+      <c r="V33" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="34" spans="22:22" x14ac:dyDescent="0.2">
+      <c r="V34" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="37" spans="22:22" x14ac:dyDescent="0.2">
+      <c r="V37" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="38" spans="22:22" x14ac:dyDescent="0.2">
+      <c r="V38" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
LTE species timeseries plots, getting new data from EDI
</commit_message>
<xml_diff>
--- a/data/functional-traits/joe-traits-lter.xlsx
+++ b/data/functional-traits/joe-traits-lter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/An/github/functional-responses/data/functional-traits/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE6A8DD-1744-1A43-B431-7F6958A81F0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A9F14B-91F6-224F-AEDE-F0531A955AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="500" windowWidth="35420" windowHeight="21060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="traits" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2613" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2668" uniqueCount="267">
   <si>
     <t>scientific_name</t>
   </si>
@@ -727,6 +727,105 @@
   </si>
   <si>
     <t>Gorostiaga, J. M. 1994. Growth and production of the red alga Gelidium sesquipedale off the Basque coast (northern Spain). Marine Biology 120:311–322.</t>
+  </si>
+  <si>
+    <t>upright or crustose</t>
+  </si>
+  <si>
+    <t>alternate</t>
+  </si>
+  <si>
+    <t>many large</t>
+  </si>
+  <si>
+    <t>stolon</t>
+  </si>
+  <si>
+    <t>Gabrielson, P. W., Widdowson, T.B., Lindstrom, S.C.. 2004. Keys to the seaweeds and seagrasses of Oregon and California.</t>
+  </si>
+  <si>
+    <t>Gabrielson and Hommersand. 1982. The morphology of Agardhiella subulata representing the Agardhielleae, a new tribe in the solieriaceae (Gigartinales, Rhodophyta)</t>
+  </si>
+  <si>
+    <t>ED assigned</t>
+  </si>
+  <si>
+    <t>AlgaeBase</t>
+  </si>
+  <si>
+    <t>former_name</t>
+  </si>
+  <si>
+    <t>former_name_source</t>
+  </si>
+  <si>
+    <t>current_name</t>
+  </si>
+  <si>
+    <t>current_name_source</t>
+  </si>
+  <si>
+    <t>Amphiroa zonata</t>
+  </si>
+  <si>
+    <t>https://ucjeps.berkeley.edu/seaweedflora/pages/californiaseaweeds.html</t>
+  </si>
+  <si>
+    <t>Acrosorium uncinatum</t>
+  </si>
+  <si>
+    <t>Cryptopleura ramosa</t>
+  </si>
+  <si>
+    <t>Algaebase</t>
+  </si>
+  <si>
+    <t>Botryoglossum farlowianum</t>
+  </si>
+  <si>
+    <t>Bossiella dichotoma</t>
+  </si>
+  <si>
+    <t>Gigartina corymbifera</t>
+  </si>
+  <si>
+    <t>Corallina chilensis</t>
+  </si>
+  <si>
+    <t>Cystoseira osmundacea</t>
+  </si>
+  <si>
+    <t>Gigartina spinosa</t>
+  </si>
+  <si>
+    <t>trichothallic</t>
+  </si>
+  <si>
+    <t>Desmarestia herbacea??</t>
+  </si>
+  <si>
+    <t>Hawkes and Scagel. 1985. The marine algae of British Columbia and northern Washington: division Rhodophyta (red algae), class Rhodophyceae, order Rhodymeniales</t>
+  </si>
+  <si>
+    <t>Fauchea fryeana</t>
+  </si>
+  <si>
+    <t>Iridaea</t>
+  </si>
+  <si>
+    <t>Some Laurencia were Janczewskia</t>
+  </si>
+  <si>
+    <t>Laurencia spectabilis</t>
+  </si>
+  <si>
+    <t>Prionitis angusta</t>
+  </si>
+  <si>
+    <t>Pseudogloiophloea confusa</t>
+  </si>
+  <si>
+    <t>Stenogramme interrupta</t>
   </si>
 </sst>
 </file>
@@ -876,7 +975,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1062,12 +1161,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1229,12 +1322,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1280,7 +1372,97 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="5" tint="-0.499984740745262"/>
@@ -1616,12 +1798,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BR55"/>
+  <dimension ref="A1:BV55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="BK1" activePane="topRight" state="frozen"/>
       <selection activeCell="A8" sqref="A8"/>
-      <selection pane="topRight" activeCell="AC3" sqref="AC3"/>
+      <selection pane="topRight" activeCell="BP14" sqref="BP14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1631,7 +1813,7 @@
     <col min="47" max="70" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1842,8 +2024,20 @@
       <c r="BR1" s="2" t="s">
         <v>188</v>
       </c>
+      <c r="BS1" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="BT1" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="BU1" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="BV1" s="2" t="s">
+        <v>245</v>
+      </c>
     </row>
-    <row r="2" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1863,7 +2057,7 @@
         <v>22</v>
       </c>
       <c r="H2" t="s">
-        <v>204</v>
+        <v>234</v>
       </c>
       <c r="I2" t="s">
         <v>133</v>
@@ -1884,19 +2078,19 @@
         <v>32</v>
       </c>
       <c r="T2" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="U2" t="s">
         <v>133</v>
       </c>
       <c r="V2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="W2" t="s">
-        <v>36</v>
+        <v>214</v>
       </c>
       <c r="X2" t="s">
-        <v>231</v>
+        <v>133</v>
       </c>
       <c r="Y2" t="s">
         <v>185</v>
@@ -1917,7 +2111,7 @@
         <v>133</v>
       </c>
       <c r="AK2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AL2" t="s">
         <v>30</v>
@@ -1940,7 +2134,7 @@
       <c r="AV2"/>
       <c r="AW2"/>
       <c r="AX2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="AY2"/>
       <c r="AZ2"/>
@@ -1950,22 +2144,22 @@
       <c r="BB2"/>
       <c r="BC2"/>
       <c r="BD2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="BE2"/>
       <c r="BF2"/>
       <c r="BG2" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="BH2"/>
       <c r="BI2"/>
       <c r="BJ2" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="BK2"/>
       <c r="BL2"/>
       <c r="BM2" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="BN2"/>
       <c r="BO2"/>
@@ -1978,8 +2172,14 @@
       <c r="BR2" t="s">
         <v>181</v>
       </c>
+      <c r="BS2" t="s">
+        <v>246</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>247</v>
+      </c>
     </row>
-    <row r="3" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -2083,10 +2283,10 @@
         <v>183</v>
       </c>
       <c r="AI3" t="s">
-        <v>61</v>
+        <v>237</v>
       </c>
       <c r="AJ3" t="s">
-        <v>133</v>
+        <v>238</v>
       </c>
       <c r="AK3" t="s">
         <v>183</v>
@@ -2122,7 +2322,7 @@
         <v>22</v>
       </c>
       <c r="AX3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="AY3"/>
       <c r="AZ3"/>
@@ -2137,12 +2337,12 @@
       <c r="BE3"/>
       <c r="BF3"/>
       <c r="BG3" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="BH3"/>
       <c r="BI3"/>
       <c r="BJ3" t="s">
-        <v>39</v>
+        <v>126</v>
       </c>
       <c r="BK3" t="s">
         <v>133</v>
@@ -2165,15 +2365,15 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>24</v>
       </c>
       <c r="B4">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>133</v>
+        <v>241</v>
       </c>
       <c r="D4" t="s">
         <v>185</v>
@@ -2214,7 +2414,7 @@
       <c r="S4" t="s">
         <v>22</v>
       </c>
-      <c r="T4" s="4" t="s">
+      <c r="T4" t="s">
         <v>29</v>
       </c>
       <c r="U4" t="s">
@@ -2260,7 +2460,7 @@
         <v>183</v>
       </c>
       <c r="AI4" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="AJ4" t="s">
         <v>133</v>
@@ -2295,7 +2495,7 @@
       <c r="AV4"/>
       <c r="AW4"/>
       <c r="AX4" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="AY4"/>
       <c r="AZ4"/>
@@ -2341,16 +2541,31 @@
       <c r="BR4" t="s">
         <v>181</v>
       </c>
+      <c r="BS4" t="s">
+        <v>248</v>
+      </c>
+      <c r="BT4" t="s">
+        <v>247</v>
+      </c>
+      <c r="BU4" t="s">
+        <v>249</v>
+      </c>
+      <c r="BV4" t="s">
+        <v>250</v>
+      </c>
     </row>
-    <row r="5" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
       <c r="B5">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>155</v>
+        <v>133</v>
+      </c>
+      <c r="D5" t="s">
+        <v>185</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -2386,7 +2601,7 @@
         <v>184</v>
       </c>
       <c r="T5" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="U5" t="s">
         <v>133</v>
@@ -2466,7 +2681,7 @@
       <c r="AV5"/>
       <c r="AW5"/>
       <c r="AX5" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="AY5"/>
       <c r="AZ5"/>
@@ -2512,13 +2727,19 @@
       <c r="BR5" t="s">
         <v>181</v>
       </c>
+      <c r="BS5" t="s">
+        <v>251</v>
+      </c>
+      <c r="BT5" t="s">
+        <v>247</v>
+      </c>
     </row>
-    <row r="6" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
       <c r="B6">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
         <v>133</v>
@@ -2530,7 +2751,7 @@
         <v>132</v>
       </c>
       <c r="H6" t="s">
-        <v>34</v>
+        <v>234</v>
       </c>
       <c r="I6" t="s">
         <v>133</v>
@@ -2553,14 +2774,14 @@
       <c r="Q6" t="s">
         <v>33</v>
       </c>
-      <c r="R6" t="s">
-        <v>132</v>
-      </c>
       <c r="T6" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="U6" t="s">
-        <v>132</v>
+        <v>133</v>
+      </c>
+      <c r="V6" t="s">
+        <v>185</v>
       </c>
       <c r="W6" t="s">
         <v>36</v>
@@ -2658,85 +2879,97 @@
       <c r="BR6" s="2" t="s">
         <v>181</v>
       </c>
+      <c r="BU6" t="s">
+        <v>252</v>
+      </c>
+      <c r="BV6" t="s">
+        <v>247</v>
+      </c>
     </row>
-    <row r="7" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>41</v>
       </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s">
-        <v>22</v>
+      <c r="B7">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7" t="s">
+        <v>185</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
       </c>
       <c r="F7" t="s">
-        <v>22</v>
+        <v>133</v>
       </c>
       <c r="G7" t="s">
-        <v>22</v>
+        <v>185</v>
       </c>
       <c r="H7" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="I7" t="s">
         <v>133</v>
       </c>
       <c r="J7" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="K7" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="N7" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="Q7" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="T7" t="s">
-        <v>22</v>
+        <v>87</v>
       </c>
       <c r="W7" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="Z7" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="AC7" t="s">
-        <v>22</v>
+        <v>117</v>
       </c>
       <c r="AF7" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="AI7" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="AL7" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="AO7" t="s">
         <v>22</v>
       </c>
       <c r="AR7" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="AU7" s="2" t="s">
         <v>22</v>
       </c>
       <c r="AX7" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="BA7" s="2" t="s">
         <v>22</v>
       </c>
       <c r="BD7" s="2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="BG7" s="2" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="BJ7" s="2" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="BM7" s="2" t="s">
         <v>22</v>
@@ -2751,7 +2984,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="8" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -2774,7 +3007,7 @@
         <v>183</v>
       </c>
       <c r="H8" t="s">
-        <v>204</v>
+        <v>234</v>
       </c>
       <c r="I8" t="s">
         <v>133</v>
@@ -2858,7 +3091,7 @@
         <v>183</v>
       </c>
       <c r="AO8" t="s">
-        <v>121</v>
+        <v>208</v>
       </c>
       <c r="AP8" t="s">
         <v>131</v>
@@ -2881,7 +3114,7 @@
       <c r="AV8"/>
       <c r="AW8"/>
       <c r="AX8" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="AY8"/>
       <c r="AZ8"/>
@@ -2928,12 +3161,12 @@
         <v>181</v>
       </c>
     </row>
-    <row r="9" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>43</v>
       </c>
       <c r="B9">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C9" t="s">
         <v>133</v>
@@ -3020,7 +3253,7 @@
         <v>22</v>
       </c>
       <c r="AX9" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="BA9" s="2" t="s">
         <v>22</v>
@@ -3058,8 +3291,14 @@
       <c r="BR9" s="2" t="s">
         <v>185</v>
       </c>
+      <c r="BS9" t="s">
+        <v>253</v>
+      </c>
+      <c r="BT9" t="s">
+        <v>247</v>
+      </c>
     </row>
-    <row r="10" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -3192,7 +3431,7 @@
       <c r="AV10"/>
       <c r="AW10"/>
       <c r="AX10" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="AY10"/>
       <c r="AZ10"/>
@@ -3239,7 +3478,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="11" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -3253,7 +3492,7 @@
         <v>185</v>
       </c>
       <c r="E11">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F11" t="s">
         <v>22</v>
@@ -3292,7 +3531,7 @@
         <v>185</v>
       </c>
       <c r="W11" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="Z11" t="s">
         <v>35</v>
@@ -3331,7 +3570,7 @@
         <v>184</v>
       </c>
       <c r="AL11" t="s">
-        <v>22</v>
+        <v>119</v>
       </c>
       <c r="AO11" t="s">
         <v>208</v>
@@ -3398,7 +3637,7 @@
       <c r="BQ11"/>
       <c r="BR11"/>
     </row>
-    <row r="12" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -3418,7 +3657,7 @@
         <v>183</v>
       </c>
       <c r="H12" t="s">
-        <v>204</v>
+        <v>234</v>
       </c>
       <c r="I12" t="s">
         <v>133</v>
@@ -3528,7 +3767,7 @@
       <c r="AV12"/>
       <c r="AW12"/>
       <c r="AX12" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="AY12"/>
       <c r="AZ12"/>
@@ -3566,7 +3805,7 @@
       <c r="BN12"/>
       <c r="BO12"/>
       <c r="BP12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="BQ12" t="s">
         <v>133</v>
@@ -3574,8 +3813,14 @@
       <c r="BR12" t="s">
         <v>181</v>
       </c>
+      <c r="BU12" t="s">
+        <v>254</v>
+      </c>
+      <c r="BV12" t="s">
+        <v>247</v>
+      </c>
     </row>
-    <row r="13" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>47</v>
       </c>
@@ -3649,10 +3894,13 @@
         <v>132</v>
       </c>
       <c r="AI13" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="AJ13" t="s">
-        <v>132</v>
+        <v>133</v>
+      </c>
+      <c r="AK13" t="s">
+        <v>185</v>
       </c>
       <c r="AL13" t="s">
         <v>51</v>
@@ -3715,7 +3963,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -3774,22 +4022,22 @@
         <v>37</v>
       </c>
       <c r="AF14" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="AI14" t="s">
         <v>61</v>
       </c>
       <c r="AL14" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="AM14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AN14" t="s">
         <v>184</v>
       </c>
       <c r="AO14" t="s">
-        <v>208</v>
+        <v>120</v>
       </c>
       <c r="AP14" t="s">
         <v>133</v>
@@ -3806,7 +4054,7 @@
       <c r="AV14"/>
       <c r="AW14"/>
       <c r="AX14" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="AY14"/>
       <c r="AZ14"/>
@@ -3840,7 +4088,7 @@
       <c r="BN14"/>
       <c r="BO14"/>
       <c r="BP14" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="BQ14" t="s">
         <v>197</v>
@@ -3849,7 +4097,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="15" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -3973,7 +4221,7 @@
       <c r="AV15"/>
       <c r="AW15"/>
       <c r="AX15" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="AY15"/>
       <c r="AZ15"/>
@@ -4020,7 +4268,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="16" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -4162,8 +4410,14 @@
       <c r="BR16" s="2" t="s">
         <v>185</v>
       </c>
+      <c r="BS16" t="s">
+        <v>255</v>
+      </c>
+      <c r="BT16" t="s">
+        <v>247</v>
+      </c>
     </row>
-    <row r="17" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>65</v>
       </c>
@@ -4306,8 +4560,14 @@
       <c r="BR17" t="s">
         <v>181</v>
       </c>
+      <c r="BS17" t="s">
+        <v>256</v>
+      </c>
+      <c r="BT17" t="s">
+        <v>247</v>
+      </c>
     </row>
-    <row r="18" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -4390,10 +4650,10 @@
         <v>132</v>
       </c>
       <c r="AO18" t="s">
-        <v>68</v>
+        <v>257</v>
       </c>
       <c r="AP18" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AR18" t="s">
         <v>32</v>
@@ -4449,8 +4709,14 @@
       <c r="BR18" s="2" t="s">
         <v>185</v>
       </c>
+      <c r="BU18" t="s">
+        <v>258</v>
+      </c>
+      <c r="BV18" t="s">
+        <v>247</v>
+      </c>
     </row>
-    <row r="19" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>71</v>
       </c>
@@ -4521,7 +4787,7 @@
         <v>32</v>
       </c>
       <c r="AI19" t="s">
-        <v>118</v>
+        <v>237</v>
       </c>
       <c r="AJ19" t="s">
         <v>133</v>
@@ -4530,7 +4796,13 @@
         <v>184</v>
       </c>
       <c r="AL19" t="s">
-        <v>30</v>
+        <v>60</v>
+      </c>
+      <c r="AM19" t="s">
+        <v>133</v>
+      </c>
+      <c r="AN19" t="s">
+        <v>182</v>
       </c>
       <c r="AO19" t="s">
         <v>121</v>
@@ -4548,7 +4820,7 @@
         <v>22</v>
       </c>
       <c r="AX19" s="2" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="BA19" s="2" t="s">
         <v>22</v>
@@ -4587,7 +4859,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="20" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>72</v>
       </c>
@@ -4721,7 +4993,7 @@
         <v>132</v>
       </c>
       <c r="BP20" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="BQ20" s="2" t="s">
         <v>200</v>
@@ -4730,7 +5002,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="21" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>74</v>
       </c>
@@ -4807,7 +5079,7 @@
         <v>185</v>
       </c>
       <c r="AC21" t="s">
-        <v>63</v>
+        <v>236</v>
       </c>
       <c r="AD21" t="s">
         <v>131</v>
@@ -4854,7 +5126,7 @@
       <c r="AV21"/>
       <c r="AW21"/>
       <c r="AX21" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="AY21"/>
       <c r="AZ21"/>
@@ -4864,17 +5136,17 @@
       <c r="BB21"/>
       <c r="BC21"/>
       <c r="BD21" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="BE21"/>
       <c r="BF21"/>
       <c r="BG21" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="BH21"/>
       <c r="BI21"/>
       <c r="BJ21" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="BK21"/>
       <c r="BL21"/>
@@ -4893,7 +5165,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="22" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>75</v>
       </c>
@@ -4906,86 +5178,86 @@
       <c r="D22" t="s">
         <v>22</v>
       </c>
-      <c r="E22" t="s">
-        <v>22</v>
+      <c r="E22">
+        <v>4</v>
       </c>
       <c r="F22" t="s">
-        <v>22</v>
+        <v>240</v>
       </c>
       <c r="G22" t="s">
-        <v>22</v>
+        <v>182</v>
       </c>
       <c r="H22" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="I22" t="s">
-        <v>22</v>
+        <v>240</v>
       </c>
       <c r="J22" t="s">
-        <v>22</v>
+        <v>182</v>
       </c>
       <c r="K22" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="N22" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="Q22" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="T22" t="s">
-        <v>22</v>
+        <v>87</v>
       </c>
       <c r="W22" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="Z22" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="AC22" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="AF22" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="AI22" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="AL22" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="AO22" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="AR22" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="AU22" s="2" t="s">
         <v>22</v>
       </c>
       <c r="AX22" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="BA22" s="2" t="s">
         <v>22</v>
       </c>
       <c r="BD22" s="2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="BG22" s="2" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="BJ22" s="2" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="BM22" s="2" t="s">
         <v>22</v>
       </c>
       <c r="BP22" s="2" t="s">
-        <v>22</v>
+        <v>190</v>
       </c>
     </row>
-    <row r="23" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>76</v>
       </c>
@@ -5008,10 +5280,10 @@
         <v>22</v>
       </c>
       <c r="H23" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="I23" t="s">
-        <v>205</v>
+        <v>240</v>
       </c>
       <c r="J23" t="s">
         <v>185</v>
@@ -5035,7 +5307,7 @@
         <v>185</v>
       </c>
       <c r="Q23" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="T23" t="s">
         <v>29</v>
@@ -5083,10 +5355,10 @@
         <v>185</v>
       </c>
       <c r="AL23" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="AO23" t="s">
-        <v>68</v>
+        <v>121</v>
       </c>
       <c r="AP23" t="s">
         <v>133</v>
@@ -5103,7 +5375,7 @@
       <c r="AV23"/>
       <c r="AW23"/>
       <c r="AX23" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="AY23"/>
       <c r="AZ23"/>
@@ -5150,7 +5422,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="24" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>77</v>
       </c>
@@ -5173,7 +5445,7 @@
         <v>22</v>
       </c>
       <c r="H24" t="s">
-        <v>114</v>
+        <v>31</v>
       </c>
       <c r="I24" t="s">
         <v>199</v>
@@ -5253,10 +5525,12 @@
       <c r="AV24"/>
       <c r="AW24"/>
       <c r="AX24" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="AY24"/>
-      <c r="AZ24"/>
+      <c r="AZ24" t="s">
+        <v>209</v>
+      </c>
       <c r="BA24" t="s">
         <v>22</v>
       </c>
@@ -5300,7 +5574,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="25" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>78</v>
       </c>
@@ -5359,13 +5633,19 @@
         <v>36</v>
       </c>
       <c r="Z25" t="s">
-        <v>35</v>
+        <v>62</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>240</v>
       </c>
       <c r="AC25" t="s">
-        <v>117</v>
+        <v>63</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>240</v>
       </c>
       <c r="AF25" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="AI25" t="s">
         <v>61</v>
@@ -5377,10 +5657,13 @@
         <v>184</v>
       </c>
       <c r="AL25" t="s">
-        <v>22</v>
+        <v>30</v>
+      </c>
+      <c r="AM25" t="s">
+        <v>240</v>
       </c>
       <c r="AO25" t="s">
-        <v>22</v>
+        <v>121</v>
       </c>
       <c r="AR25" t="s">
         <v>32</v>
@@ -5391,10 +5674,14 @@
       <c r="AV25"/>
       <c r="AW25"/>
       <c r="AX25" t="s">
-        <v>22</v>
-      </c>
-      <c r="AY25"/>
-      <c r="AZ25"/>
+        <v>27</v>
+      </c>
+      <c r="AY25" t="s">
+        <v>259</v>
+      </c>
+      <c r="AZ25" t="s">
+        <v>209</v>
+      </c>
       <c r="BA25" t="s">
         <v>22</v>
       </c>
@@ -5437,25 +5724,31 @@
       <c r="BR25" t="s">
         <v>181</v>
       </c>
+      <c r="BS25" t="s">
+        <v>260</v>
+      </c>
+      <c r="BT25" t="s">
+        <v>247</v>
+      </c>
     </row>
-    <row r="26" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>79</v>
       </c>
-      <c r="B26" t="s">
-        <v>22</v>
+      <c r="B26">
+        <v>7</v>
       </c>
       <c r="C26" t="s">
-        <v>22</v>
+        <v>155</v>
       </c>
       <c r="D26" t="s">
-        <v>22</v>
-      </c>
-      <c r="E26" t="s">
-        <v>22</v>
+        <v>183</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>22</v>
+        <v>240</v>
       </c>
       <c r="G26" t="s">
         <v>22</v>
@@ -5470,58 +5763,70 @@
         <v>183</v>
       </c>
       <c r="K26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N26" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="Q26" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="T26" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="W26" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="Z26" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="AC26" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="AF26" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="AI26" t="s">
-        <v>22</v>
+        <v>73</v>
+      </c>
+      <c r="AJ26" t="s">
+        <v>133</v>
+      </c>
+      <c r="AK26" t="s">
+        <v>184</v>
       </c>
       <c r="AL26" t="s">
-        <v>22</v>
+        <v>119</v>
+      </c>
+      <c r="AM26" t="s">
+        <v>133</v>
       </c>
       <c r="AO26" t="s">
-        <v>22</v>
+        <v>68</v>
+      </c>
+      <c r="AP26" t="s">
+        <v>133</v>
       </c>
       <c r="AR26" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="AU26" s="2" t="s">
         <v>22</v>
       </c>
       <c r="AX26" s="2" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="BA26" s="2" t="s">
         <v>22</v>
       </c>
       <c r="BD26" s="2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="BG26" s="2" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="BJ26" s="2" t="s">
-        <v>22</v>
+        <v>127</v>
       </c>
       <c r="BM26" s="2" t="s">
         <v>22</v>
@@ -5530,7 +5835,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>80</v>
       </c>
@@ -5634,7 +5939,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="28" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>81</v>
       </c>
@@ -5738,7 +6043,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="29" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -5833,7 +6138,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>83</v>
       </c>
@@ -5846,11 +6151,11 @@
       <c r="D30" t="s">
         <v>184</v>
       </c>
-      <c r="E30" t="s">
-        <v>22</v>
+      <c r="E30">
+        <v>3</v>
       </c>
       <c r="F30" t="s">
-        <v>22</v>
+        <v>240</v>
       </c>
       <c r="G30" t="s">
         <v>22</v>
@@ -5933,13 +6238,13 @@
       <c r="AV30"/>
       <c r="AW30"/>
       <c r="AX30" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="AY30" t="s">
-        <v>213</v>
+        <v>240</v>
       </c>
       <c r="AZ30" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="BA30" t="s">
         <v>28</v>
@@ -5988,12 +6293,12 @@
         <v>184</v>
       </c>
     </row>
-    <row r="31" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>84</v>
       </c>
       <c r="B31">
-        <v>18</v>
+        <v>200</v>
       </c>
       <c r="C31" t="s">
         <v>133</v>
@@ -6104,7 +6409,7 @@
         <v>183</v>
       </c>
       <c r="AO31" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AP31" t="s">
         <v>215</v>
@@ -6121,10 +6426,14 @@
       <c r="AV31"/>
       <c r="AW31"/>
       <c r="AX31" t="s">
-        <v>22</v>
-      </c>
-      <c r="AY31"/>
-      <c r="AZ31"/>
+        <v>27</v>
+      </c>
+      <c r="AY31" t="s">
+        <v>240</v>
+      </c>
+      <c r="AZ31" t="s">
+        <v>182</v>
+      </c>
       <c r="BA31" t="s">
         <v>22</v>
       </c>
@@ -6168,12 +6477,12 @@
         <v>184</v>
       </c>
     </row>
-    <row r="32" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>85</v>
       </c>
       <c r="B32">
-        <v>70</v>
+        <v>25</v>
       </c>
       <c r="C32" t="s">
         <v>133</v>
@@ -6301,7 +6610,7 @@
       <c r="AV32"/>
       <c r="AW32"/>
       <c r="AX32" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="AY32"/>
       <c r="AZ32"/>
@@ -6348,12 +6657,12 @@
         <v>181</v>
       </c>
     </row>
-    <row r="33" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>86</v>
       </c>
       <c r="B33">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C33" t="s">
         <v>133</v>
@@ -6377,10 +6686,13 @@
         <v>132</v>
       </c>
       <c r="N33" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O33" t="s">
-        <v>132</v>
+        <v>133</v>
+      </c>
+      <c r="P33" t="s">
+        <v>184</v>
       </c>
       <c r="Q33" t="s">
         <v>32</v>
@@ -6491,12 +6803,12 @@
         <v>185</v>
       </c>
     </row>
-    <row r="34" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>88</v>
       </c>
       <c r="B34">
-        <v>15</v>
+        <v>140</v>
       </c>
       <c r="C34" t="s">
         <v>133</v>
@@ -6544,7 +6856,7 @@
         <v>32</v>
       </c>
       <c r="T34" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="U34" t="s">
         <v>133</v>
@@ -6559,7 +6871,7 @@
         <v>62</v>
       </c>
       <c r="AC34" t="s">
-        <v>63</v>
+        <v>117</v>
       </c>
       <c r="AF34" t="s">
         <v>32</v>
@@ -6606,7 +6918,7 @@
       <c r="AV34"/>
       <c r="AW34"/>
       <c r="AX34" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="AY34"/>
       <c r="AZ34"/>
@@ -6616,7 +6928,7 @@
       <c r="BB34"/>
       <c r="BC34"/>
       <c r="BD34" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="BE34"/>
       <c r="BF34"/>
@@ -6652,8 +6964,14 @@
       <c r="BR34" t="s">
         <v>181</v>
       </c>
+      <c r="BS34" t="s">
+        <v>261</v>
+      </c>
+      <c r="BT34" t="s">
+        <v>247</v>
+      </c>
     </row>
-    <row r="35" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>89</v>
       </c>
@@ -6703,7 +7021,7 @@
         <v>132</v>
       </c>
       <c r="W35" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="X35" t="s">
         <v>132</v>
@@ -6799,7 +7117,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="36" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>92</v>
       </c>
@@ -6942,7 +7260,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="37" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>93</v>
       </c>
@@ -7019,7 +7337,13 @@
         <v>184</v>
       </c>
       <c r="AL37" t="s">
-        <v>30</v>
+        <v>60</v>
+      </c>
+      <c r="AM37" t="s">
+        <v>133</v>
+      </c>
+      <c r="AN37" t="s">
+        <v>184</v>
       </c>
       <c r="AO37" t="s">
         <v>121</v>
@@ -7039,7 +7363,7 @@
       <c r="AV37"/>
       <c r="AW37"/>
       <c r="AX37" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="AY37"/>
       <c r="AZ37"/>
@@ -7077,13 +7401,19 @@
       <c r="BR37" s="1" t="s">
         <v>181</v>
       </c>
+      <c r="BS37" t="s">
+        <v>262</v>
+      </c>
+      <c r="BT37" t="s">
+        <v>247</v>
+      </c>
     </row>
-    <row r="38" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>94</v>
       </c>
       <c r="B38">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="C38" t="s">
         <v>133</v>
@@ -7223,8 +7553,14 @@
       <c r="BR38" s="3" t="s">
         <v>181</v>
       </c>
+      <c r="BS38" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="BT38" t="s">
+        <v>247</v>
+      </c>
     </row>
-    <row r="39" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>95</v>
       </c>
@@ -7271,7 +7607,7 @@
         <v>132</v>
       </c>
       <c r="W39" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="X39" t="s">
         <v>132</v>
@@ -7283,7 +7619,7 @@
         <v>132</v>
       </c>
       <c r="AC39" t="s">
-        <v>63</v>
+        <v>236</v>
       </c>
       <c r="AD39" t="s">
         <v>132</v>
@@ -7361,7 +7697,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>96</v>
       </c>
@@ -7467,7 +7803,7 @@
       <c r="AV40"/>
       <c r="AW40"/>
       <c r="AX40" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="AY40"/>
       <c r="AZ40"/>
@@ -7482,7 +7818,7 @@
       <c r="BE40"/>
       <c r="BF40"/>
       <c r="BG40" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="BH40"/>
       <c r="BI40"/>
@@ -7506,7 +7842,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="41" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>97</v>
       </c>
@@ -7514,7 +7850,7 @@
         <v>40</v>
       </c>
       <c r="C41" t="s">
-        <v>133</v>
+        <v>222</v>
       </c>
       <c r="D41" t="s">
         <v>185</v>
@@ -7550,10 +7886,10 @@
         <v>32</v>
       </c>
       <c r="T41" t="s">
-        <v>29</v>
+        <v>235</v>
       </c>
       <c r="U41" t="s">
-        <v>133</v>
+        <v>239</v>
       </c>
       <c r="V41" t="s">
         <v>185</v>
@@ -7562,7 +7898,7 @@
         <v>54</v>
       </c>
       <c r="X41" t="s">
-        <v>133</v>
+        <v>239</v>
       </c>
       <c r="Y41" t="s">
         <v>184</v>
@@ -7577,67 +7913,82 @@
         <v>32</v>
       </c>
       <c r="AI41" t="s">
-        <v>118</v>
+        <v>61</v>
       </c>
       <c r="AJ41" t="s">
-        <v>133</v>
+        <v>239</v>
       </c>
       <c r="AK41" t="s">
         <v>185</v>
       </c>
       <c r="AL41" t="s">
-        <v>30</v>
+        <v>119</v>
+      </c>
+      <c r="AM41" t="s">
+        <v>222</v>
       </c>
       <c r="AO41" t="s">
         <v>121</v>
       </c>
       <c r="AP41" t="s">
-        <v>133</v>
+        <v>222</v>
       </c>
       <c r="AQ41" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="AR41" t="s">
         <v>32</v>
       </c>
-      <c r="AU41" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AX41" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="BA41" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="BD41" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="BG41" s="2" t="s">
+      <c r="AU41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV41"/>
+      <c r="AW41"/>
+      <c r="AX41" t="s">
+        <v>27</v>
+      </c>
+      <c r="AY41"/>
+      <c r="AZ41"/>
+      <c r="BA41" t="s">
+        <v>22</v>
+      </c>
+      <c r="BB41"/>
+      <c r="BC41"/>
+      <c r="BD41" t="s">
+        <v>32</v>
+      </c>
+      <c r="BE41"/>
+      <c r="BF41"/>
+      <c r="BG41" t="s">
         <v>64</v>
       </c>
-      <c r="BH41" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="BI41" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="BJ41" s="2" t="s">
+      <c r="BH41" t="s">
+        <v>133</v>
+      </c>
+      <c r="BI41" t="s">
+        <v>184</v>
+      </c>
+      <c r="BJ41" t="s">
         <v>128</v>
       </c>
-      <c r="BM41" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="BP41" s="2" t="s">
+      <c r="BK41"/>
+      <c r="BL41"/>
+      <c r="BM41" t="s">
+        <v>22</v>
+      </c>
+      <c r="BN41"/>
+      <c r="BO41"/>
+      <c r="BP41" t="s">
         <v>190</v>
       </c>
-      <c r="BQ41" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="BR41" s="3" t="s">
+      <c r="BQ41" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="BR41" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="42" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>98</v>
       </c>
@@ -7743,7 +8094,7 @@
       <c r="AV42"/>
       <c r="AW42"/>
       <c r="AX42" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="AY42"/>
       <c r="AZ42"/>
@@ -7790,12 +8141,12 @@
         <v>185</v>
       </c>
     </row>
-    <row r="43" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>99</v>
       </c>
       <c r="B43">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="C43" t="s">
         <v>132</v>
@@ -7807,10 +8158,10 @@
         <v>132</v>
       </c>
       <c r="H43" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="I43" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K43" t="s">
         <v>32</v>
@@ -7933,7 +8284,7 @@
         <v>132</v>
       </c>
       <c r="BP43" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="BQ43" s="3" t="s">
         <v>133</v>
@@ -7942,7 +8293,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="44" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>100</v>
       </c>
@@ -8051,7 +8402,7 @@
       <c r="AV44"/>
       <c r="AW44"/>
       <c r="AX44" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="AY44"/>
       <c r="AZ44"/>
@@ -8098,12 +8449,12 @@
         <v>185</v>
       </c>
     </row>
-    <row r="45" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>101</v>
       </c>
       <c r="B45">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C45" t="s">
         <v>133</v>
@@ -8204,7 +8555,7 @@
       <c r="AV45"/>
       <c r="AW45"/>
       <c r="AX45" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="AY45"/>
       <c r="AZ45"/>
@@ -8250,8 +8601,14 @@
       <c r="BR45" t="s">
         <v>181</v>
       </c>
+      <c r="BS45" t="s">
+        <v>264</v>
+      </c>
+      <c r="BT45" t="s">
+        <v>247</v>
+      </c>
     </row>
-    <row r="46" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>102</v>
       </c>
@@ -8310,7 +8667,7 @@
         <v>132</v>
       </c>
       <c r="AC46" t="s">
-        <v>63</v>
+        <v>236</v>
       </c>
       <c r="AD46" t="s">
         <v>132</v>
@@ -8394,7 +8751,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="47" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>103</v>
       </c>
@@ -8465,7 +8822,7 @@
         <v>32</v>
       </c>
       <c r="AI47" t="s">
-        <v>118</v>
+        <v>237</v>
       </c>
       <c r="AJ47" t="s">
         <v>133</v>
@@ -8500,7 +8857,7 @@
       <c r="AV47"/>
       <c r="AW47"/>
       <c r="AX47" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="AY47"/>
       <c r="AZ47"/>
@@ -8547,7 +8904,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="48" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>104</v>
       </c>
@@ -8585,7 +8942,10 @@
         <v>133</v>
       </c>
       <c r="N48" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="O48" t="s">
+        <v>133</v>
       </c>
       <c r="Q48" t="s">
         <v>32</v>
@@ -8647,7 +9007,7 @@
       <c r="AV48"/>
       <c r="AW48"/>
       <c r="AX48" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="AY48"/>
       <c r="AZ48"/>
@@ -8657,17 +9017,17 @@
       <c r="BB48"/>
       <c r="BC48"/>
       <c r="BD48" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="BE48"/>
       <c r="BF48"/>
       <c r="BG48" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="BH48"/>
       <c r="BI48"/>
       <c r="BJ48" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="BK48"/>
       <c r="BL48"/>
@@ -8686,7 +9046,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="49" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>105</v>
       </c>
@@ -8823,7 +9183,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>106</v>
       </c>
@@ -8966,7 +9326,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="51" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>107</v>
       </c>
@@ -9046,7 +9406,7 @@
         <v>184</v>
       </c>
       <c r="AL51" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="AM51" t="s">
         <v>224</v>
@@ -9072,7 +9432,7 @@
       <c r="AV51"/>
       <c r="AW51"/>
       <c r="AX51" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="AY51"/>
       <c r="AZ51"/>
@@ -9087,7 +9447,7 @@
       <c r="BE51"/>
       <c r="BF51"/>
       <c r="BG51" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="BH51" t="s">
         <v>133</v>
@@ -9118,8 +9478,14 @@
       <c r="BR51" t="s">
         <v>181</v>
       </c>
+      <c r="BS51" t="s">
+        <v>265</v>
+      </c>
+      <c r="BT51" t="s">
+        <v>247</v>
+      </c>
     </row>
-    <row r="52" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>108</v>
       </c>
@@ -9196,7 +9562,7 @@
         <v>185</v>
       </c>
       <c r="AO52" t="s">
-        <v>208</v>
+        <v>68</v>
       </c>
       <c r="AP52" t="s">
         <v>133</v>
@@ -9213,7 +9579,7 @@
       <c r="AV52"/>
       <c r="AW52"/>
       <c r="AX52" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="AY52"/>
       <c r="AZ52"/>
@@ -9260,7 +9626,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="53" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>109</v>
       </c>
@@ -9360,7 +9726,7 @@
       <c r="AV53"/>
       <c r="AW53"/>
       <c r="AX53" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="AY53"/>
       <c r="AZ53"/>
@@ -9406,8 +9772,14 @@
       <c r="BR53" t="s">
         <v>181</v>
       </c>
+      <c r="BS53" t="s">
+        <v>266</v>
+      </c>
+      <c r="BT53" t="s">
+        <v>247</v>
+      </c>
     </row>
-    <row r="54" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>110</v>
       </c>
@@ -9504,7 +9876,7 @@
       <c r="AV54"/>
       <c r="AW54"/>
       <c r="AX54" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="AY54"/>
       <c r="AZ54"/>
@@ -9555,7 +9927,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="55" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>111</v>
       </c>
@@ -9652,7 +10024,7 @@
       <c r="AV55"/>
       <c r="AW55"/>
       <c r="AX55" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="AY55"/>
       <c r="AZ55"/>
@@ -9701,168 +10073,17 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:BR55" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="A1:XFD3 A4:AT5 AU4:XFD14 A6:B6 E6:AT6 A7:AT14 A15:XFD15 AV16:XFD35 A16:AU55 AV36:BP38 BS36:XFD38 AV39:XFD40 AV41:BP41 BS41:XFD41 AV42:XFD42 AV43:BP43 BR43:XFD43 AV44:XFD55 A56:XFD1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="A56:XFD1048576 BW1:XFD55">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+      <formula>"NA"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:BV5 E6:BR6 BU6:BV6 A6:B7 D7:BV7 A8:BV15 AV16:BV35 A16:AU55 AV36:BP38 BS36:BV38 AV39:BV40 AV41:BP41 BS41:BV41 AV42:BV42 AV43:BP43 BR43:BV43 AV44:BV55">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="25">
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Heads up!" error="You entered unexpected data. Double check your values, or change the validation. Hit &quot;yes&quot; if you want to keep the value, or &quot;no&quot; if you need to fix it." xr:uid="{0D295492-5677-8741-A437-15B078D10DFC}">
-          <x14:formula1>
-            <xm:f>validation!$A$2:$A$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>E2:E55</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A1D2B872-180E-104C-88E0-AD9CB96AF424}">
-          <x14:formula1>
-            <xm:f>validation!$C$2:$C$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>K2:K55</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5CAAFBA6-CEA6-D846-806A-386F70B07362}">
-          <x14:formula1>
-            <xm:f>validation!$D$2:$D$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>N2:N55</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A9BDCB57-8114-7F43-9BBA-D60C744A9D6C}">
-          <x14:formula1>
-            <xm:f>validation!$E$2:$E$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>Q2:Q55</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BDF6956C-FD4F-5745-9BAD-4F06078E2E6F}">
-          <x14:formula1>
-            <xm:f>validation!$H$2:$H$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>Z2:Z55</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E4EB3441-CF23-C14C-BAC2-28B561FE24AD}">
-          <x14:formula1>
-            <xm:f>validation!$I$2:$I$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>AC2:AC55</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CD1FE25B-8863-C846-AE44-D9E3987DFA82}">
-          <x14:formula1>
-            <xm:f>validation!$J$2:$J$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>AF2:AF55</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9D444779-5FED-B848-94B4-7EFE6006FD15}">
-          <x14:formula1>
-            <xm:f>validation!$K$2:$K$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>AI2:AI55</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DC67A632-EA9E-7A40-8755-32102AF144FB}">
-          <x14:formula1>
-            <xm:f>validation!$L$2:$L$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>AL2:AL55</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{81D61B1D-0FA3-CB4C-8530-70367251F5E1}">
-          <x14:formula1>
-            <xm:f>validation!$O$2:$O$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>AU2:AU55</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A7BEABB9-1932-7148-B0A3-687CB0A5D620}">
-          <x14:formula1>
-            <xm:f>validation!$N$2:$N$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>AR2:AR55</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DDB9593D-F45F-2F42-95C8-5B128D52BD22}">
-          <x14:formula1>
-            <xm:f>validation!$P$2:$P$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>AX2:AX55</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{060B551E-A192-0148-A213-14D881D4CC05}">
-          <x14:formula1>
-            <xm:f>validation!$Q$2:$Q$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>BA2:BA55</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{76497AF8-48BF-134E-AA9C-F80965198A52}">
-          <x14:formula1>
-            <xm:f>validation!$R$2:$R$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>BD2:BD55</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2E2A3ED5-0BBA-BD4B-9F2E-FF364DF72375}">
-          <x14:formula1>
-            <xm:f>validation!$S$2:$S$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>BG2:BG55</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F479D1C0-58D7-0048-B4FB-3639CD857DBE}">
-          <x14:formula1>
-            <xm:f>validation!$T$2:$T$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>BJ2:BJ55</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C56351E5-2996-8F4E-91D5-F8C7F747062B}">
-          <x14:formula1>
-            <xm:f>validation!$U$2:$U$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>BM2:BM55</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{34C0EFFE-4DDA-3A46-A1DD-552B7D37CB4A}">
-          <x14:formula1>
-            <xm:f>validation!$X$2:$X$8</xm:f>
-          </x14:formula1>
-          <xm:sqref>BP2:BP55</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5C3892B1-C038-8C41-B6A1-4128954F5A8F}">
-          <x14:formula1>
-            <xm:f>validation!$B$2:$B$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>H2:H55</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2F8867B2-872C-324C-A280-3CF467007787}">
-          <x14:formula1>
-            <xm:f>validation!$F$2:$F$10</xm:f>
-          </x14:formula1>
-          <xm:sqref>T2:T55</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6725AB14-EC0B-444D-9D39-6EEE353F0A42}">
-          <x14:formula1>
-            <xm:f>validation!$W$2:$W$8</xm:f>
-          </x14:formula1>
-          <xm:sqref>BR42:BR55 BR39:BR40 AN2:AN55 BR2:BR35 BO2:BO55 BL2:BL55 BI2:BI55 BF2:BF55 BC2:BC55 AZ2:AZ55 AW2:AW55 AT2:AT55 AQ2:AQ55 D2:D55 AK2:AK55 AH2:AH55 AE2:AE55 AB2:AB55 Y2:Y55 V2:V55 S2:S55 P2:P55 J2:J55 M2:M55 G2:G55</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C3AC2B56-3C29-FF4A-917A-FE404650079C}">
-          <x14:formula1>
-            <xm:f>validation!$M$2:$M$8</xm:f>
-          </x14:formula1>
-          <xm:sqref>AO2:AO55</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9ADE18B9-CF42-6545-A97C-880DB242063B}">
-          <x14:formula1>
-            <xm:f>validation!$G$2:$G$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>W2:W55</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C96C3B9F-507F-B84A-84DE-52C47F8B8221}">
-          <x14:formula1>
-            <xm:f>validation!$V$2:$V$42</xm:f>
-          </x14:formula1>
-          <xm:sqref>U2:U55 BH2:BH55 BE2:BE55 BB2:BB55 AY2:AY55 AV2:AV55 BN2:BN55 C2:C55 AJ2:AJ55 AG2:AG55 AD2:AD55 AA2:AA55 X2:X55 F2:F55 R2:R55 O2:O55 I2:I55 BK2:BK55 L2:L55 AP2:AP55 AM2:AM55 AS2:AS55</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EBBD6087-25C7-A94D-A5DC-6224CEDACC0A}">
-          <x14:formula1>
-            <xm:f>validation!$V$2:$V$48</xm:f>
-          </x14:formula1>
-          <xm:sqref>BQ44:BQ55 BQ42 BQ39:BQ40 BQ2:BQ35</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -9870,7 +10091,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAABEA72-4450-9143-B9EE-F8CB7C81A2E6}">
   <dimension ref="A1:X38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="V35" sqref="V35"/>
     </sheetView>
   </sheetViews>
@@ -10448,7 +10669,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L1:X1">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>